<commit_message>
Automatisches Update vom 2025-06-04_22-18
</commit_message>
<xml_diff>
--- a/NotenAllSuS.xlsx
+++ b/NotenAllSuS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bslinz3-my.sharepoint.com/personal/m_knoll_bs-linz3_ac_at/Documents/Sonstiges/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bslinz3-my.sharepoint.com/personal/m_knoll_bs-linz3_ac_at/Documents/Sonstiges/NotenListeGesamt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{148FE47A-C517-4B6B-ACEE-1181345031EE}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89EB8416-1AC8-4270-92BC-3B3EB7C81DDA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
   </bookViews>
@@ -6889,9 +6889,6 @@
       <sheetData sheetId="4"/>
       <sheetData sheetId="5">
         <row r="2">
-          <cell r="A2">
-            <v>204606</v>
-          </cell>
           <cell r="B2" t="str">
             <v>VT-N_24 25_3cCVT</v>
           </cell>
@@ -9465,6 +9462,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9786,7 +9787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9400B600-DABD-46EA-8221-46FAC4AE4807}">
   <dimension ref="A1:CI120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A109" sqref="A109"/>
     </sheetView>
   </sheetViews>
@@ -10381,7 +10382,7 @@
       </c>
       <c r="CH2" s="1">
         <f ca="1">NOW()</f>
-        <v>45812.901018750003</v>
+        <v>45812.913298263891</v>
       </c>
     </row>
     <row r="3" spans="1:87" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Automatisches Update vom 2025-06-05_12-00
</commit_message>
<xml_diff>
--- a/NotenAllSuS.xlsx
+++ b/NotenAllSuS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bslinz3-my.sharepoint.com/personal/m_knoll_bs-linz3_ac_at/Documents/Sonstiges/NotenListeGesamt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89EB8416-1AC8-4270-92BC-3B3EB7C81DDA}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CAB34CB-18D4-4702-8217-82D1451ACBA4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2717" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2718" uniqueCount="345">
   <si>
     <t>StudentCode</t>
   </si>
@@ -1074,6 +1074,9 @@
   <si>
     <t>Endnote: 1 Sehr guter Mathematiker!</t>
   </si>
+  <si>
+    <t>Test_2</t>
+  </si>
 </sst>
 </file>
 
@@ -9787,8 +9790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9400B600-DABD-46EA-8221-46FAC4AE4807}">
   <dimension ref="A1:CI120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10106,19 +10109,17 @@
       <c r="O2">
         <v>5</v>
       </c>
-      <c r="P2">
-        <v>0</v>
+      <c r="P2" t="s">
+        <v>344</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:BS2" si="1">P2</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R2">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="Q2:BS2" si="1">R2</f>
         <v>0</v>
       </c>
       <c r="T2">
@@ -10382,7 +10383,7 @@
       </c>
       <c r="CH2" s="1">
         <f ca="1">NOW()</f>
-        <v>45812.942176041666</v>
+        <v>45812.949498379632</v>
       </c>
     </row>
     <row r="3" spans="1:87" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Automatisches Update vom 2025-06-10_10-26
</commit_message>
<xml_diff>
--- a/NotenAllSuS.xlsx
+++ b/NotenAllSuS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CAB34CB-18D4-4702-8217-82D1451ACBA4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
+    <workbookView xWindow="75" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
   </bookViews>
   <sheets>
     <sheet name="NotenAllSuS" sheetId="1" r:id="rId1"/>
@@ -9467,10 +9467,6 @@
 </externalLink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -9794,14 +9790,14 @@
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10061,7 +10057,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101010</v>
       </c>
@@ -10119,7 +10115,7 @@
         <v>0</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="Q2:BS2" si="1">R2</f>
+        <f t="shared" ref="S2:BS2" si="1">R2</f>
         <v>0</v>
       </c>
       <c r="T2">
@@ -10383,10 +10379,10 @@
       </c>
       <c r="CH2" s="1">
         <f ca="1">NOW()</f>
-        <v>45812.949498379632</v>
+        <v>45818.423642013891</v>
       </c>
     </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>101010</v>
       </c>
@@ -10647,7 +10643,7 @@
       </c>
       <c r="CI3" s="1"/>
     </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>101010</v>
       </c>
@@ -10907,7 +10903,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>238868</v>
       </c>
@@ -11167,7 +11163,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>239513</v>
       </c>
@@ -11427,7 +11423,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>238869</v>
       </c>
@@ -11687,7 +11683,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>238938</v>
       </c>
@@ -11947,7 +11943,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>235241</v>
       </c>
@@ -12207,7 +12203,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>234202</v>
       </c>
@@ -12467,7 +12463,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>239517</v>
       </c>
@@ -12727,7 +12723,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>235188</v>
       </c>
@@ -12987,7 +12983,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>238873</v>
       </c>
@@ -13247,7 +13243,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>235970</v>
       </c>
@@ -13507,7 +13503,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>233683</v>
       </c>
@@ -13767,7 +13763,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:87" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>238629</v>
       </c>
@@ -14027,7 +14023,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>235163</v>
       </c>
@@ -14287,7 +14283,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>236320</v>
       </c>
@@ -14547,7 +14543,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>235239</v>
       </c>
@@ -14807,7 +14803,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>240757</v>
       </c>
@@ -15067,7 +15063,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>241467</v>
       </c>
@@ -15327,7 +15323,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>227176</v>
       </c>
@@ -15587,7 +15583,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>237814</v>
       </c>
@@ -15847,7 +15843,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>234162</v>
       </c>
@@ -16107,7 +16103,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>234166</v>
       </c>
@@ -16367,7 +16363,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>234165</v>
       </c>
@@ -16627,7 +16623,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>234159</v>
       </c>
@@ -16887,7 +16883,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>234146</v>
       </c>
@@ -17147,7 +17143,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>234156</v>
       </c>
@@ -17407,7 +17403,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>234303</v>
       </c>
@@ -17667,7 +17663,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>234160</v>
       </c>
@@ -17927,7 +17923,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>225611</v>
       </c>
@@ -18187,7 +18183,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="33" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>234157</v>
       </c>
@@ -18447,7 +18443,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>234158</v>
       </c>
@@ -18707,7 +18703,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>234155</v>
       </c>
@@ -18967,7 +18963,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>234147</v>
       </c>
@@ -19227,7 +19223,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>234144</v>
       </c>
@@ -19487,7 +19483,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>242412</v>
       </c>
@@ -19747,7 +19743,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="39" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>241867</v>
       </c>
@@ -20007,7 +20003,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="40" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>242615</v>
       </c>
@@ -20267,7 +20263,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="41" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>236774</v>
       </c>
@@ -20527,7 +20523,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="42" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>242616</v>
       </c>
@@ -20787,7 +20783,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>242617</v>
       </c>
@@ -21047,7 +21043,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="44" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>727090</v>
       </c>
@@ -21307,7 +21303,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="45" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>235211</v>
       </c>
@@ -21567,7 +21563,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="46" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>241945</v>
       </c>
@@ -21827,7 +21823,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>238493</v>
       </c>
@@ -22087,7 +22083,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="48" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>242050</v>
       </c>
@@ -22347,7 +22343,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="49" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>238954</v>
       </c>
@@ -22607,7 +22603,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="50" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>239023</v>
       </c>
@@ -22867,7 +22863,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="51" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>238267</v>
       </c>
@@ -23127,7 +23123,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>239024</v>
       </c>
@@ -23387,7 +23383,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="53" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>238314</v>
       </c>
@@ -23647,7 +23643,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="54" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>247308</v>
       </c>
@@ -23907,7 +23903,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="55" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>240051</v>
       </c>
@@ -24167,7 +24163,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="56" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>246501</v>
       </c>
@@ -24427,7 +24423,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="57" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>245566</v>
       </c>
@@ -24687,7 +24683,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="58" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>245509</v>
       </c>
@@ -24947,7 +24943,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="59" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>245510</v>
       </c>
@@ -25207,7 +25203,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="60" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>241923</v>
       </c>
@@ -25467,7 +25463,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="61" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>238486</v>
       </c>
@@ -25727,7 +25723,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="62" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>243487</v>
       </c>
@@ -25987,7 +25983,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="63" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>234145</v>
       </c>
@@ -26247,7 +26243,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="64" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>225004</v>
       </c>
@@ -26507,7 +26503,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="65" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>244511</v>
       </c>
@@ -26767,7 +26763,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="66" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>224044</v>
       </c>
@@ -27027,7 +27023,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="67" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>241871</v>
       </c>
@@ -27287,7 +27283,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="68" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>242618</v>
       </c>
@@ -27547,7 +27543,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="69" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>245041</v>
       </c>
@@ -27807,7 +27803,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="70" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>242619</v>
       </c>
@@ -28067,7 +28063,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="71" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>242620</v>
       </c>
@@ -28327,7 +28323,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="72" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>242622</v>
       </c>
@@ -28587,7 +28583,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="73" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>242621</v>
       </c>
@@ -28847,7 +28843,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="74" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>242623</v>
       </c>
@@ -29107,7 +29103,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="75" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>241872</v>
       </c>
@@ -29367,7 +29363,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="76" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>242625</v>
       </c>
@@ -29627,7 +29623,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="77" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>244014</v>
       </c>
@@ -29887,7 +29883,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="78" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>242627</v>
       </c>
@@ -30147,7 +30143,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="79" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>242631</v>
       </c>
@@ -30407,7 +30403,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="80" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>243487</v>
       </c>
@@ -30667,7 +30663,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="81" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>244511</v>
       </c>
@@ -30927,7 +30923,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="82" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>242618</v>
       </c>
@@ -31187,7 +31183,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="83" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>245041</v>
       </c>
@@ -31447,7 +31443,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="84" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>242619</v>
       </c>
@@ -31707,7 +31703,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="85" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>242622</v>
       </c>
@@ -31967,7 +31963,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="86" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>242621</v>
       </c>
@@ -32227,7 +32223,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="87" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>242623</v>
       </c>
@@ -32487,7 +32483,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="88" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>242631</v>
       </c>
@@ -32747,7 +32743,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="89" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A89">
         <f>[1]Uebertrag!A2</f>
         <v>204606</v>
@@ -33093,7 +33089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A90">
         <f>[1]Uebertrag!A3</f>
         <v>225128</v>
@@ -33439,7 +33435,7 @@
         <v>Ol zu spät</v>
       </c>
     </row>
-    <row r="91" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A91">
         <f>[1]Uebertrag!A4</f>
         <v>229524</v>
@@ -33785,7 +33781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A92">
         <f>[1]Uebertrag!A5</f>
         <v>225129</v>
@@ -34131,7 +34127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A93">
         <f>[1]Uebertrag!A6</f>
         <v>228179</v>
@@ -34477,7 +34473,7 @@
         <v>Abgabe Photometer fehlt</v>
       </c>
     </row>
-    <row r="94" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A94">
         <f>[1]Uebertrag!A7</f>
         <v>227298</v>
@@ -34823,7 +34819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A95">
         <f>[1]Uebertrag!A8</f>
         <v>225126</v>
@@ -35169,7 +35165,7 @@
         <v>Kaugummi, PSA!; Öl nicht abgegeben</v>
       </c>
     </row>
-    <row r="96" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A96">
         <f>[1]Uebertrag!A9</f>
         <v>226369</v>
@@ -35515,7 +35511,7 @@
         <v>Abgabe Photometer, Polarimetrie fehlt, Unsachgemäßer Aufbau + Nichtbeachten grundlegender Sicherheitsvorgaben (dichte Schliffverbindungen, sichere Befestigung). Fehlende Eigenkontrolle vor Versuchsbeginn.  Schaffung einer vermeidbaren Gefahrensituation durch Austritt brennbarer Dämpfe und Überhitzung.</v>
       </c>
     </row>
-    <row r="97" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A97">
         <f>[1]Uebertrag!A10</f>
         <v>226368</v>
@@ -35861,7 +35857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A98">
         <f>[1]Uebertrag!A11</f>
         <v>228085</v>
@@ -36207,7 +36203,7 @@
         <v>Acetylsalizylsäure fehlerhafte Abgabe daher noch nicht bewertet</v>
       </c>
     </row>
-    <row r="99" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A99">
         <f>[2]HTMLÜbertrag!A3</f>
         <v>225936</v>
@@ -36553,7 +36549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A100">
         <f>[2]HTMLÜbertrag!A6</f>
         <v>225954</v>
@@ -36899,7 +36895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A101">
         <f>[2]HTMLÜbertrag!A8</f>
         <v>225939</v>
@@ -37245,7 +37241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A102">
         <f>[2]HTMLÜbertrag!A9</f>
         <v>226813</v>
@@ -37591,7 +37587,7 @@
         <v>Mitschrift sehr gut</v>
       </c>
     </row>
-    <row r="103" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A103">
         <f>[2]HTMLÜbertrag!A11</f>
         <v>225129</v>
@@ -37937,7 +37933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A104">
         <f>[2]HTMLÜbertrag!A12</f>
         <v>228179</v>
@@ -38283,7 +38279,7 @@
         <v>BSP v S. 298+299 fehlen,</v>
       </c>
     </row>
-    <row r="105" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A105">
         <f>[2]HTMLÜbertrag!A13</f>
         <v>225935</v>
@@ -38629,7 +38625,7 @@
         <v>Mitschrift sehr gut</v>
       </c>
     </row>
-    <row r="106" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A106">
         <f>[2]HTMLÜbertrag!A15</f>
         <v>225934</v>
@@ -38975,7 +38971,7 @@
         <v>Mitschrift sehr gut</v>
       </c>
     </row>
-    <row r="107" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A107">
         <f>[2]HTMLÜbertrag!A16</f>
         <v>225126</v>
@@ -39321,7 +39317,7 @@
         <v>Mitschrift in Ordnung</v>
       </c>
     </row>
-    <row r="108" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A108">
         <f>[2]HTMLÜbertrag!A18</f>
         <v>225955</v>
@@ -39667,7 +39663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>204606</v>
       </c>
@@ -40012,7 +40008,7 @@
         <v xml:space="preserve">Motivierter Schüler mit guten Fragen. Entspannen Sie sich und bleiben Sie ehrgeizig. </v>
       </c>
     </row>
-    <row r="110" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>225128</v>
       </c>
@@ -40357,7 +40353,7 @@
         <v>Beteiligt sich oft während des Unterrichts, oft fehlt aber der Feinschliff bei den Aussagen zu einer MA Note 1. Lernen Sie mit.</v>
       </c>
     </row>
-    <row r="111" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>225129</v>
       </c>
@@ -40702,7 +40698,7 @@
         <v>Gute leistung beim zweiten Test! Lernen Sie mit.</v>
       </c>
     </row>
-    <row r="112" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>228179</v>
       </c>
@@ -41047,7 +41043,7 @@
         <v>Beteiligen Sie sich mehr am Unterricht und Lernen Sie mit. Ich werde Sie in diesem Fach mahnen.</v>
       </c>
     </row>
-    <row r="113" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>227298</v>
       </c>
@@ -41392,7 +41388,7 @@
         <v xml:space="preserve">Aufgestufft. Ihre Formulierung und Kombinationen sind gut. Versuchen Sie bei der Sache zu bleiben. </v>
       </c>
     </row>
-    <row r="114" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>225934</v>
       </c>
@@ -41737,7 +41733,7 @@
         <v>Sie sind bemüht. Alernen Sie mit und genauer.</v>
       </c>
     </row>
-    <row r="115" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>225126</v>
       </c>
@@ -42082,7 +42078,7 @@
         <v>Bitte lernen Sie mit +genauer</v>
       </c>
     </row>
-    <row r="116" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>226369</v>
       </c>
@@ -42427,7 +42423,7 @@
         <v>Oft haben Sie wirklich gute Antworten auf meine Fragen. Trauen Sie sich mehr zu! Versuchen Sie täglich VT zu lernen</v>
       </c>
     </row>
-    <row r="117" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>225955</v>
       </c>
@@ -42772,7 +42768,7 @@
         <v>Die Antworten während des Unterrichts sind oft noch zu wenig genau für eine 1 in der MA</v>
       </c>
     </row>
-    <row r="118" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>226368</v>
       </c>
@@ -43117,7 +43113,7 @@
         <v>Formulierungskönig! Lernen Sie mit und genau.</v>
       </c>
     </row>
-    <row r="120" spans="1:86" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:86" x14ac:dyDescent="0.25">
       <c r="B120" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatisches Update vom 2025-06-10_11-18
</commit_message>
<xml_diff>
--- a/NotenAllSuS.xlsx
+++ b/NotenAllSuS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bslinz3-my.sharepoint.com/personal/m_knoll_bs-linz3_ac_at/Documents/Sonstiges/NotenListeGesamt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6CAB34CB-18D4-4702-8217-82D1451ACBA4}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{379FB828-E368-4B48-8220-804C9F630640}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
   </bookViews>
   <sheets>
     <sheet name="NotenAllSuS" sheetId="1" r:id="rId1"/>
@@ -1645,13 +1645,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C2">
-            <v>1.1499999999999999</v>
+            <v>1.1333333333333333</v>
           </cell>
           <cell r="D2">
             <v>0</v>
           </cell>
           <cell r="E2">
-            <v>1.1499999999999999</v>
+            <v>1.1333333333333333</v>
           </cell>
           <cell r="F2" t="str">
             <v>Viskosität</v>
@@ -1699,7 +1699,7 @@
             <v>Fehling \  red. Verbindung</v>
           </cell>
           <cell r="U2">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="V2" t="str">
             <v>Flü Flü Extraktion</v>
@@ -1905,13 +1905,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C3">
-            <v>1.2615714285714286</v>
+            <v>1.2455000000000001</v>
           </cell>
           <cell r="D3">
             <v>0</v>
           </cell>
           <cell r="E3">
-            <v>1.2615714285714286</v>
+            <v>1.2455000000000001</v>
           </cell>
           <cell r="F3" t="str">
             <v>Viskosität</v>
@@ -1959,7 +1959,7 @@
             <v>Fehling \  red. Verbindung</v>
           </cell>
           <cell r="U3">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="V3" t="str">
             <v>Flü Flü Extraktion</v>
@@ -2165,13 +2165,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C4">
-            <v>1.1499999999999999</v>
+            <v>1.1285714285714286</v>
           </cell>
           <cell r="D4">
             <v>0</v>
           </cell>
           <cell r="E4">
-            <v>1.1499999999999999</v>
+            <v>1.1285714285714286</v>
           </cell>
           <cell r="F4" t="str">
             <v>Viskosität</v>
@@ -2219,7 +2219,7 @@
             <v>Fehling \  red. Verbindung</v>
           </cell>
           <cell r="U4">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="V4" t="str">
             <v>Flü Flü Extraktion</v>
@@ -2425,13 +2425,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C5">
-            <v>1.2666666666666666</v>
+            <v>1.24</v>
           </cell>
           <cell r="D5">
             <v>0</v>
           </cell>
           <cell r="E5">
-            <v>1.2666666666666666</v>
+            <v>1.24</v>
           </cell>
           <cell r="F5" t="str">
             <v>Viskosität</v>
@@ -2479,7 +2479,7 @@
             <v>Fehling \  red. Verbindung</v>
           </cell>
           <cell r="U5">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="V5" t="str">
             <v>Flü Flü Extraktion</v>
@@ -2685,13 +2685,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C6">
-            <v>1.633</v>
+            <v>1.5615714285714286</v>
           </cell>
           <cell r="D6">
             <v>0</v>
           </cell>
           <cell r="E6">
-            <v>1.633</v>
+            <v>1.5615714285714286</v>
           </cell>
           <cell r="F6" t="str">
             <v>Viskosität</v>
@@ -2739,7 +2739,7 @@
             <v>Fehling \  red. Verbindung</v>
           </cell>
           <cell r="U6">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="V6" t="str">
             <v>Flü Flü Extraktion</v>
@@ -2945,13 +2945,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C7">
-            <v>1.1499999999999999</v>
+            <v>1.1333333333333333</v>
           </cell>
           <cell r="D7">
             <v>0</v>
           </cell>
           <cell r="E7">
-            <v>1.1499999999999999</v>
+            <v>1.1333333333333333</v>
           </cell>
           <cell r="F7" t="str">
             <v>Viskosität</v>
@@ -2999,7 +2999,7 @@
             <v>Fehling \  red. Verbindung</v>
           </cell>
           <cell r="U7">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="V7" t="str">
             <v>Flü Flü Extraktion</v>
@@ -3205,13 +3205,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C8">
-            <v>1.4670000000000001</v>
+            <v>1.4384285714285714</v>
           </cell>
           <cell r="D8">
             <v>0</v>
           </cell>
           <cell r="E8">
-            <v>1.4670000000000001</v>
+            <v>1.4384285714285714</v>
           </cell>
           <cell r="F8" t="str">
             <v>Viskosität</v>
@@ -3259,7 +3259,7 @@
             <v>Fehling \  red. Verbindung</v>
           </cell>
           <cell r="U8">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="V8" t="str">
             <v>Flü Flü Extraktion</v>
@@ -3465,13 +3465,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C9">
-            <v>2.0169999999999999</v>
+            <v>1.9670000000000001</v>
           </cell>
           <cell r="D9">
             <v>0</v>
           </cell>
           <cell r="E9">
-            <v>2.0169999999999999</v>
+            <v>1.9670000000000001</v>
           </cell>
           <cell r="F9" t="str">
             <v>Viskosität</v>
@@ -3519,7 +3519,7 @@
             <v>Fehling \  red. Verbindung</v>
           </cell>
           <cell r="U9">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="V9" t="str">
             <v>Flü Flü Extraktion</v>
@@ -3725,13 +3725,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C10">
-            <v>1.18</v>
+            <v>1.1499999999999999</v>
           </cell>
           <cell r="D10">
             <v>0</v>
           </cell>
           <cell r="E10">
-            <v>1.18</v>
+            <v>1.1499999999999999</v>
           </cell>
           <cell r="F10" t="str">
             <v>Viskosität</v>
@@ -3779,7 +3779,7 @@
             <v>Fehling \  red. Verbindung</v>
           </cell>
           <cell r="U10">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="V10" t="str">
             <v>Flü Flü Extraktion</v>
@@ -3985,13 +3985,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C11">
-            <v>1.2250000000000001</v>
+            <v>1.2</v>
           </cell>
           <cell r="D11">
             <v>0</v>
           </cell>
           <cell r="E11">
-            <v>1.2250000000000001</v>
+            <v>1.2</v>
           </cell>
           <cell r="F11" t="str">
             <v>Viskosität</v>
@@ -4039,7 +4039,7 @@
             <v>Fehling \  red. Verbindung</v>
           </cell>
           <cell r="U11">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="V11" t="str">
             <v>Flü Flü Extraktion</v>
@@ -4272,13 +4272,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C3">
-            <v>1.6</v>
+            <v>1.83</v>
           </cell>
           <cell r="D3">
             <v>3</v>
           </cell>
           <cell r="E3">
-            <v>2.44</v>
+            <v>2.5299999999999998</v>
           </cell>
           <cell r="F3" t="str">
             <v>W1</v>
@@ -4370,11 +4370,11 @@
           <cell r="AI3">
             <v>1</v>
           </cell>
-          <cell r="AJ3">
-            <v>6</v>
+          <cell r="AJ3" t="str">
+            <v>Phyaik.Berechn.</v>
           </cell>
           <cell r="AK3">
-            <v>0</v>
+            <v>3</v>
           </cell>
           <cell r="AL3">
             <v>7</v>
@@ -4532,13 +4532,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C6">
-            <v>1.4</v>
+            <v>2</v>
           </cell>
           <cell r="D6">
             <v>3.2</v>
           </cell>
           <cell r="E6">
-            <v>2.48</v>
+            <v>2.72</v>
           </cell>
           <cell r="F6" t="str">
             <v>W1</v>
@@ -4630,11 +4630,11 @@
           <cell r="AI6">
             <v>3</v>
           </cell>
-          <cell r="AJ6">
-            <v>6</v>
+          <cell r="AJ6" t="str">
+            <v>Phyaik.Berechn.</v>
           </cell>
           <cell r="AK6">
-            <v>0</v>
+            <v>5</v>
           </cell>
           <cell r="AL6">
             <v>7</v>
@@ -4792,13 +4792,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C8">
-            <v>1.2</v>
+            <v>1.83</v>
           </cell>
           <cell r="D8">
             <v>2.4</v>
           </cell>
           <cell r="E8">
-            <v>1.92</v>
+            <v>2.17</v>
           </cell>
           <cell r="F8" t="str">
             <v>W1</v>
@@ -4890,11 +4890,11 @@
           <cell r="AI8">
             <v>1</v>
           </cell>
-          <cell r="AJ8">
-            <v>6</v>
+          <cell r="AJ8" t="str">
+            <v>Phyaik.Berechn.</v>
           </cell>
           <cell r="AK8">
-            <v>0</v>
+            <v>5</v>
           </cell>
           <cell r="AL8">
             <v>7</v>
@@ -5052,13 +5052,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C9">
-            <v>3.6</v>
+            <v>3.67</v>
           </cell>
           <cell r="D9">
             <v>3.1</v>
           </cell>
           <cell r="E9">
-            <v>3.3</v>
+            <v>3.33</v>
           </cell>
           <cell r="F9" t="str">
             <v>W1</v>
@@ -5150,11 +5150,11 @@
           <cell r="AI9">
             <v>3</v>
           </cell>
-          <cell r="AJ9">
-            <v>6</v>
+          <cell r="AJ9" t="str">
+            <v>Phyaik.Berechn.</v>
           </cell>
           <cell r="AK9">
-            <v>0</v>
+            <v>4</v>
           </cell>
           <cell r="AL9">
             <v>7</v>
@@ -5312,13 +5312,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C11">
-            <v>1.6</v>
+            <v>2</v>
           </cell>
           <cell r="D11">
             <v>2.4</v>
           </cell>
           <cell r="E11">
-            <v>2.08</v>
+            <v>2.2400000000000002</v>
           </cell>
           <cell r="F11" t="str">
             <v>W1</v>
@@ -5410,11 +5410,11 @@
           <cell r="AI11">
             <v>2</v>
           </cell>
-          <cell r="AJ11">
-            <v>6</v>
+          <cell r="AJ11" t="str">
+            <v>Phyaik.Berechn.</v>
           </cell>
           <cell r="AK11">
-            <v>0</v>
+            <v>4</v>
           </cell>
           <cell r="AL11">
             <v>7</v>
@@ -5572,13 +5572,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C12">
-            <v>2.67</v>
+            <v>3</v>
           </cell>
           <cell r="D12">
             <v>3.4</v>
           </cell>
           <cell r="E12">
-            <v>3.11</v>
+            <v>3.24</v>
           </cell>
           <cell r="F12" t="str">
             <v>W1</v>
@@ -5670,11 +5670,11 @@
           <cell r="AI12">
             <v>1</v>
           </cell>
-          <cell r="AJ12">
-            <v>6</v>
+          <cell r="AJ12" t="str">
+            <v>Phyaik.Berechn.</v>
           </cell>
           <cell r="AK12">
-            <v>0</v>
+            <v>5</v>
           </cell>
           <cell r="AL12">
             <v>7</v>
@@ -5832,13 +5832,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C13">
-            <v>2.4</v>
+            <v>2.5</v>
           </cell>
           <cell r="D13">
             <v>3.7</v>
           </cell>
           <cell r="E13">
-            <v>3.18</v>
+            <v>3.22</v>
           </cell>
           <cell r="F13" t="str">
             <v>W1</v>
@@ -5930,11 +5930,11 @@
           <cell r="AI13">
             <v>1</v>
           </cell>
-          <cell r="AJ13">
-            <v>6</v>
+          <cell r="AJ13" t="str">
+            <v>Phyaik.Berechn.</v>
           </cell>
           <cell r="AK13">
-            <v>0</v>
+            <v>3</v>
           </cell>
           <cell r="AL13">
             <v>7</v>
@@ -6092,13 +6092,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C15">
-            <v>2.8</v>
+            <v>3</v>
           </cell>
           <cell r="D15">
             <v>3</v>
           </cell>
           <cell r="E15">
-            <v>2.92</v>
+            <v>3</v>
           </cell>
           <cell r="F15" t="str">
             <v>W1</v>
@@ -6190,11 +6190,11 @@
           <cell r="AI15">
             <v>1</v>
           </cell>
-          <cell r="AJ15">
-            <v>6</v>
+          <cell r="AJ15" t="str">
+            <v>Phyaik.Berechn.</v>
           </cell>
           <cell r="AK15">
-            <v>0</v>
+            <v>4</v>
           </cell>
           <cell r="AL15">
             <v>7</v>
@@ -6352,13 +6352,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C16">
-            <v>2.8</v>
+            <v>3.17</v>
           </cell>
           <cell r="D16">
             <v>4.3</v>
           </cell>
           <cell r="E16">
-            <v>3.7</v>
+            <v>3.85</v>
           </cell>
           <cell r="F16" t="str">
             <v>W1</v>
@@ -6450,11 +6450,11 @@
           <cell r="AI16">
             <v>2</v>
           </cell>
-          <cell r="AJ16">
-            <v>6</v>
+          <cell r="AJ16" t="str">
+            <v>Phyaik.Berechn.</v>
           </cell>
           <cell r="AK16">
-            <v>0</v>
+            <v>5</v>
           </cell>
           <cell r="AL16">
             <v>7</v>
@@ -6612,13 +6612,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C18">
-            <v>1.2</v>
+            <v>1.5</v>
           </cell>
           <cell r="D18">
             <v>2.2000000000000002</v>
           </cell>
           <cell r="E18">
-            <v>1.8</v>
+            <v>1.92</v>
           </cell>
           <cell r="F18" t="str">
             <v>W1</v>
@@ -6710,11 +6710,11 @@
           <cell r="AI18">
             <v>1</v>
           </cell>
-          <cell r="AJ18">
-            <v>6</v>
+          <cell r="AJ18" t="str">
+            <v>Phyaik.Berechn.</v>
           </cell>
           <cell r="AK18">
-            <v>0</v>
+            <v>3</v>
           </cell>
           <cell r="AL18">
             <v>7</v>
@@ -9465,6 +9465,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9786,7 +9790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9400B600-DABD-46EA-8221-46FAC4AE4807}">
   <dimension ref="A1:CI120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U88" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -10379,7 +10383,7 @@
       </c>
       <c r="CH2" s="1">
         <f ca="1">NOW()</f>
-        <v>45818.423642013891</v>
+        <v>45818.465395949075</v>
       </c>
     </row>
     <row r="3" spans="1:87" x14ac:dyDescent="0.25">
@@ -32754,7 +32758,7 @@
       </c>
       <c r="C89">
         <f>[1]Uebertrag!C2</f>
-        <v>1.1499999999999999</v>
+        <v>1.1333333333333333</v>
       </c>
       <c r="D89">
         <f>[1]Uebertrag!D2</f>
@@ -32762,7 +32766,7 @@
       </c>
       <c r="E89">
         <f>[1]Uebertrag!E2</f>
-        <v>1.1499999999999999</v>
+        <v>1.1333333333333333</v>
       </c>
       <c r="F89" t="str">
         <f>[1]Uebertrag!F2</f>
@@ -32826,7 +32830,7 @@
       </c>
       <c r="U89">
         <f>[1]Uebertrag!U2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V89" t="str">
         <f>[1]Uebertrag!V2</f>
@@ -33100,7 +33104,7 @@
       </c>
       <c r="C90">
         <f>[1]Uebertrag!C3</f>
-        <v>1.2615714285714286</v>
+        <v>1.2455000000000001</v>
       </c>
       <c r="D90">
         <f>[1]Uebertrag!D3</f>
@@ -33108,7 +33112,7 @@
       </c>
       <c r="E90">
         <f>[1]Uebertrag!E3</f>
-        <v>1.2615714285714286</v>
+        <v>1.2455000000000001</v>
       </c>
       <c r="F90" t="str">
         <f>[1]Uebertrag!F3</f>
@@ -33172,7 +33176,7 @@
       </c>
       <c r="U90">
         <f>[1]Uebertrag!U3</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V90" t="str">
         <f>[1]Uebertrag!V3</f>
@@ -33446,7 +33450,7 @@
       </c>
       <c r="C91">
         <f>[1]Uebertrag!C4</f>
-        <v>1.1499999999999999</v>
+        <v>1.1285714285714286</v>
       </c>
       <c r="D91">
         <f>[1]Uebertrag!D4</f>
@@ -33454,7 +33458,7 @@
       </c>
       <c r="E91">
         <f>[1]Uebertrag!E4</f>
-        <v>1.1499999999999999</v>
+        <v>1.1285714285714286</v>
       </c>
       <c r="F91" t="str">
         <f>[1]Uebertrag!F4</f>
@@ -33518,7 +33522,7 @@
       </c>
       <c r="U91">
         <f>[1]Uebertrag!U4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V91" t="str">
         <f>[1]Uebertrag!V4</f>
@@ -33792,7 +33796,7 @@
       </c>
       <c r="C92">
         <f>[1]Uebertrag!C5</f>
-        <v>1.2666666666666666</v>
+        <v>1.24</v>
       </c>
       <c r="D92">
         <f>[1]Uebertrag!D5</f>
@@ -33800,7 +33804,7 @@
       </c>
       <c r="E92">
         <f>[1]Uebertrag!E5</f>
-        <v>1.2666666666666666</v>
+        <v>1.24</v>
       </c>
       <c r="F92" t="str">
         <f>[1]Uebertrag!F5</f>
@@ -33864,7 +33868,7 @@
       </c>
       <c r="U92">
         <f>[1]Uebertrag!U5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V92" t="str">
         <f>[1]Uebertrag!V5</f>
@@ -34138,7 +34142,7 @@
       </c>
       <c r="C93">
         <f>[1]Uebertrag!C6</f>
-        <v>1.633</v>
+        <v>1.5615714285714286</v>
       </c>
       <c r="D93">
         <f>[1]Uebertrag!D6</f>
@@ -34146,7 +34150,7 @@
       </c>
       <c r="E93">
         <f>[1]Uebertrag!E6</f>
-        <v>1.633</v>
+        <v>1.5615714285714286</v>
       </c>
       <c r="F93" t="str">
         <f>[1]Uebertrag!F6</f>
@@ -34210,7 +34214,7 @@
       </c>
       <c r="U93">
         <f>[1]Uebertrag!U6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V93" t="str">
         <f>[1]Uebertrag!V6</f>
@@ -34484,7 +34488,7 @@
       </c>
       <c r="C94">
         <f>[1]Uebertrag!C7</f>
-        <v>1.1499999999999999</v>
+        <v>1.1333333333333333</v>
       </c>
       <c r="D94">
         <f>[1]Uebertrag!D7</f>
@@ -34492,7 +34496,7 @@
       </c>
       <c r="E94">
         <f>[1]Uebertrag!E7</f>
-        <v>1.1499999999999999</v>
+        <v>1.1333333333333333</v>
       </c>
       <c r="F94" t="str">
         <f>[1]Uebertrag!F7</f>
@@ -34556,7 +34560,7 @@
       </c>
       <c r="U94">
         <f>[1]Uebertrag!U7</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V94" t="str">
         <f>[1]Uebertrag!V7</f>
@@ -34830,7 +34834,7 @@
       </c>
       <c r="C95">
         <f>[1]Uebertrag!C8</f>
-        <v>1.4670000000000001</v>
+        <v>1.4384285714285714</v>
       </c>
       <c r="D95">
         <f>[1]Uebertrag!D8</f>
@@ -34838,7 +34842,7 @@
       </c>
       <c r="E95">
         <f>[1]Uebertrag!E8</f>
-        <v>1.4670000000000001</v>
+        <v>1.4384285714285714</v>
       </c>
       <c r="F95" t="str">
         <f>[1]Uebertrag!F8</f>
@@ -34902,7 +34906,7 @@
       </c>
       <c r="U95">
         <f>[1]Uebertrag!U8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V95" t="str">
         <f>[1]Uebertrag!V8</f>
@@ -35176,7 +35180,7 @@
       </c>
       <c r="C96">
         <f>[1]Uebertrag!C9</f>
-        <v>2.0169999999999999</v>
+        <v>1.9670000000000001</v>
       </c>
       <c r="D96">
         <f>[1]Uebertrag!D9</f>
@@ -35184,7 +35188,7 @@
       </c>
       <c r="E96">
         <f>[1]Uebertrag!E9</f>
-        <v>2.0169999999999999</v>
+        <v>1.9670000000000001</v>
       </c>
       <c r="F96" t="str">
         <f>[1]Uebertrag!F9</f>
@@ -35248,7 +35252,7 @@
       </c>
       <c r="U96">
         <f>[1]Uebertrag!U9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V96" t="str">
         <f>[1]Uebertrag!V9</f>
@@ -35522,7 +35526,7 @@
       </c>
       <c r="C97">
         <f>[1]Uebertrag!C10</f>
-        <v>1.18</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="D97">
         <f>[1]Uebertrag!D10</f>
@@ -35530,7 +35534,7 @@
       </c>
       <c r="E97">
         <f>[1]Uebertrag!E10</f>
-        <v>1.18</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="F97" t="str">
         <f>[1]Uebertrag!F10</f>
@@ -35594,7 +35598,7 @@
       </c>
       <c r="U97">
         <f>[1]Uebertrag!U10</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V97" t="str">
         <f>[1]Uebertrag!V10</f>
@@ -35868,7 +35872,7 @@
       </c>
       <c r="C98">
         <f>[1]Uebertrag!C11</f>
-        <v>1.2250000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="D98">
         <f>[1]Uebertrag!D11</f>
@@ -35876,7 +35880,7 @@
       </c>
       <c r="E98">
         <f>[1]Uebertrag!E11</f>
-        <v>1.2250000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="F98" t="str">
         <f>[1]Uebertrag!F11</f>
@@ -35940,7 +35944,7 @@
       </c>
       <c r="U98">
         <f>[1]Uebertrag!U11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V98" t="str">
         <f>[1]Uebertrag!V11</f>
@@ -36214,7 +36218,7 @@
       </c>
       <c r="C99">
         <f>[2]HTMLÜbertrag!C3</f>
-        <v>1.6</v>
+        <v>1.83</v>
       </c>
       <c r="D99">
         <f>[2]HTMLÜbertrag!D3</f>
@@ -36222,7 +36226,7 @@
       </c>
       <c r="E99">
         <f>[2]HTMLÜbertrag!E3</f>
-        <v>2.44</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="F99" t="str">
         <f>[2]HTMLÜbertrag!F3</f>
@@ -36344,13 +36348,13 @@
         <f>[2]HTMLÜbertrag!AI3</f>
         <v>1</v>
       </c>
-      <c r="AJ99">
+      <c r="AJ99" t="str">
         <f>[2]HTMLÜbertrag!AJ3</f>
-        <v>6</v>
+        <v>Phyaik.Berechn.</v>
       </c>
       <c r="AK99">
         <f>[2]HTMLÜbertrag!AK3</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL99">
         <f>[2]HTMLÜbertrag!AL3</f>
@@ -36560,7 +36564,7 @@
       </c>
       <c r="C100">
         <f>[2]HTMLÜbertrag!C6</f>
-        <v>1.4</v>
+        <v>2</v>
       </c>
       <c r="D100">
         <f>[2]HTMLÜbertrag!D6</f>
@@ -36568,7 +36572,7 @@
       </c>
       <c r="E100">
         <f>[2]HTMLÜbertrag!E6</f>
-        <v>2.48</v>
+        <v>2.72</v>
       </c>
       <c r="F100" t="str">
         <f>[2]HTMLÜbertrag!F6</f>
@@ -36690,13 +36694,13 @@
         <f>[2]HTMLÜbertrag!AI6</f>
         <v>3</v>
       </c>
-      <c r="AJ100">
+      <c r="AJ100" t="str">
         <f>[2]HTMLÜbertrag!AJ6</f>
-        <v>6</v>
+        <v>Phyaik.Berechn.</v>
       </c>
       <c r="AK100">
         <f>[2]HTMLÜbertrag!AK6</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL100">
         <f>[2]HTMLÜbertrag!AL6</f>
@@ -36906,7 +36910,7 @@
       </c>
       <c r="C101">
         <f>[2]HTMLÜbertrag!C8</f>
-        <v>1.2</v>
+        <v>1.83</v>
       </c>
       <c r="D101">
         <f>[2]HTMLÜbertrag!D8</f>
@@ -36914,7 +36918,7 @@
       </c>
       <c r="E101">
         <f>[2]HTMLÜbertrag!E8</f>
-        <v>1.92</v>
+        <v>2.17</v>
       </c>
       <c r="F101" t="str">
         <f>[2]HTMLÜbertrag!F8</f>
@@ -37036,13 +37040,13 @@
         <f>[2]HTMLÜbertrag!AI8</f>
         <v>1</v>
       </c>
-      <c r="AJ101">
+      <c r="AJ101" t="str">
         <f>[2]HTMLÜbertrag!AJ8</f>
-        <v>6</v>
+        <v>Phyaik.Berechn.</v>
       </c>
       <c r="AK101">
         <f>[2]HTMLÜbertrag!AK8</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL101">
         <f>[2]HTMLÜbertrag!AL8</f>
@@ -37252,7 +37256,7 @@
       </c>
       <c r="C102">
         <f>[2]HTMLÜbertrag!C9</f>
-        <v>3.6</v>
+        <v>3.67</v>
       </c>
       <c r="D102">
         <f>[2]HTMLÜbertrag!D9</f>
@@ -37260,7 +37264,7 @@
       </c>
       <c r="E102">
         <f>[2]HTMLÜbertrag!E9</f>
-        <v>3.3</v>
+        <v>3.33</v>
       </c>
       <c r="F102" t="str">
         <f>[2]HTMLÜbertrag!F9</f>
@@ -37382,13 +37386,13 @@
         <f>[2]HTMLÜbertrag!AI9</f>
         <v>3</v>
       </c>
-      <c r="AJ102">
+      <c r="AJ102" t="str">
         <f>[2]HTMLÜbertrag!AJ9</f>
-        <v>6</v>
+        <v>Phyaik.Berechn.</v>
       </c>
       <c r="AK102">
         <f>[2]HTMLÜbertrag!AK9</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL102">
         <f>[2]HTMLÜbertrag!AL9</f>
@@ -37598,7 +37602,7 @@
       </c>
       <c r="C103">
         <f>[2]HTMLÜbertrag!C11</f>
-        <v>1.6</v>
+        <v>2</v>
       </c>
       <c r="D103">
         <f>[2]HTMLÜbertrag!D11</f>
@@ -37606,7 +37610,7 @@
       </c>
       <c r="E103">
         <f>[2]HTMLÜbertrag!E11</f>
-        <v>2.08</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="F103" t="str">
         <f>[2]HTMLÜbertrag!F11</f>
@@ -37728,13 +37732,13 @@
         <f>[2]HTMLÜbertrag!AI11</f>
         <v>2</v>
       </c>
-      <c r="AJ103">
+      <c r="AJ103" t="str">
         <f>[2]HTMLÜbertrag!AJ11</f>
-        <v>6</v>
+        <v>Phyaik.Berechn.</v>
       </c>
       <c r="AK103">
         <f>[2]HTMLÜbertrag!AK11</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL103">
         <f>[2]HTMLÜbertrag!AL11</f>
@@ -37944,7 +37948,7 @@
       </c>
       <c r="C104">
         <f>[2]HTMLÜbertrag!C12</f>
-        <v>2.67</v>
+        <v>3</v>
       </c>
       <c r="D104">
         <f>[2]HTMLÜbertrag!D12</f>
@@ -37952,7 +37956,7 @@
       </c>
       <c r="E104">
         <f>[2]HTMLÜbertrag!E12</f>
-        <v>3.11</v>
+        <v>3.24</v>
       </c>
       <c r="F104" t="str">
         <f>[2]HTMLÜbertrag!F12</f>
@@ -38074,13 +38078,13 @@
         <f>[2]HTMLÜbertrag!AI12</f>
         <v>1</v>
       </c>
-      <c r="AJ104">
+      <c r="AJ104" t="str">
         <f>[2]HTMLÜbertrag!AJ12</f>
-        <v>6</v>
+        <v>Phyaik.Berechn.</v>
       </c>
       <c r="AK104">
         <f>[2]HTMLÜbertrag!AK12</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL104">
         <f>[2]HTMLÜbertrag!AL12</f>
@@ -38290,7 +38294,7 @@
       </c>
       <c r="C105">
         <f>[2]HTMLÜbertrag!C13</f>
-        <v>2.4</v>
+        <v>2.5</v>
       </c>
       <c r="D105">
         <f>[2]HTMLÜbertrag!D13</f>
@@ -38298,7 +38302,7 @@
       </c>
       <c r="E105">
         <f>[2]HTMLÜbertrag!E13</f>
-        <v>3.18</v>
+        <v>3.22</v>
       </c>
       <c r="F105" t="str">
         <f>[2]HTMLÜbertrag!F13</f>
@@ -38420,13 +38424,13 @@
         <f>[2]HTMLÜbertrag!AI13</f>
         <v>1</v>
       </c>
-      <c r="AJ105">
+      <c r="AJ105" t="str">
         <f>[2]HTMLÜbertrag!AJ13</f>
-        <v>6</v>
+        <v>Phyaik.Berechn.</v>
       </c>
       <c r="AK105">
         <f>[2]HTMLÜbertrag!AK13</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL105">
         <f>[2]HTMLÜbertrag!AL13</f>
@@ -38636,7 +38640,7 @@
       </c>
       <c r="C106">
         <f>[2]HTMLÜbertrag!C15</f>
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="D106">
         <f>[2]HTMLÜbertrag!D15</f>
@@ -38644,7 +38648,7 @@
       </c>
       <c r="E106">
         <f>[2]HTMLÜbertrag!E15</f>
-        <v>2.92</v>
+        <v>3</v>
       </c>
       <c r="F106" t="str">
         <f>[2]HTMLÜbertrag!F15</f>
@@ -38766,13 +38770,13 @@
         <f>[2]HTMLÜbertrag!AI15</f>
         <v>1</v>
       </c>
-      <c r="AJ106">
+      <c r="AJ106" t="str">
         <f>[2]HTMLÜbertrag!AJ15</f>
-        <v>6</v>
+        <v>Phyaik.Berechn.</v>
       </c>
       <c r="AK106">
         <f>[2]HTMLÜbertrag!AK15</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AL106">
         <f>[2]HTMLÜbertrag!AL15</f>
@@ -38982,7 +38986,7 @@
       </c>
       <c r="C107">
         <f>[2]HTMLÜbertrag!C16</f>
-        <v>2.8</v>
+        <v>3.17</v>
       </c>
       <c r="D107">
         <f>[2]HTMLÜbertrag!D16</f>
@@ -38990,7 +38994,7 @@
       </c>
       <c r="E107">
         <f>[2]HTMLÜbertrag!E16</f>
-        <v>3.7</v>
+        <v>3.85</v>
       </c>
       <c r="F107" t="str">
         <f>[2]HTMLÜbertrag!F16</f>
@@ -39112,13 +39116,13 @@
         <f>[2]HTMLÜbertrag!AI16</f>
         <v>2</v>
       </c>
-      <c r="AJ107">
+      <c r="AJ107" t="str">
         <f>[2]HTMLÜbertrag!AJ16</f>
-        <v>6</v>
+        <v>Phyaik.Berechn.</v>
       </c>
       <c r="AK107">
         <f>[2]HTMLÜbertrag!AK16</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AL107">
         <f>[2]HTMLÜbertrag!AL16</f>
@@ -39328,7 +39332,7 @@
       </c>
       <c r="C108">
         <f>[2]HTMLÜbertrag!C18</f>
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="D108">
         <f>[2]HTMLÜbertrag!D18</f>
@@ -39336,7 +39340,7 @@
       </c>
       <c r="E108">
         <f>[2]HTMLÜbertrag!E18</f>
-        <v>1.8</v>
+        <v>1.92</v>
       </c>
       <c r="F108" t="str">
         <f>[2]HTMLÜbertrag!F18</f>
@@ -39458,13 +39462,13 @@
         <f>[2]HTMLÜbertrag!AI18</f>
         <v>1</v>
       </c>
-      <c r="AJ108">
+      <c r="AJ108" t="str">
         <f>[2]HTMLÜbertrag!AJ18</f>
-        <v>6</v>
+        <v>Phyaik.Berechn.</v>
       </c>
       <c r="AK108">
         <f>[2]HTMLÜbertrag!AK18</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL108">
         <f>[2]HTMLÜbertrag!AL18</f>

</xml_diff>

<commit_message>
Automatisches Update vom 2025-06-11_17-34
</commit_message>
<xml_diff>
--- a/NotenAllSuS.xlsx
+++ b/NotenAllSuS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{379FB828-E368-4B48-8220-804C9F630640}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
+    <workbookView xWindow="0" yWindow="3210" windowWidth="21600" windowHeight="11385" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
   </bookViews>
   <sheets>
     <sheet name="NotenAllSuS" sheetId="1" r:id="rId1"/>
@@ -2945,13 +2945,13 @@
             <v>3cCVTLab_GrKNoll</v>
           </cell>
           <cell r="C7">
-            <v>1.1333333333333333</v>
+            <v>1.3338333333333334</v>
           </cell>
           <cell r="D7">
             <v>0</v>
           </cell>
           <cell r="E7">
-            <v>1.1333333333333333</v>
+            <v>1.3338333333333334</v>
           </cell>
           <cell r="F7" t="str">
             <v>Viskosität</v>
@@ -3149,7 +3149,7 @@
             <v>Sicherheitsaspekte</v>
           </cell>
           <cell r="BS7">
-            <v>1</v>
+            <v>2</v>
           </cell>
           <cell r="BT7" t="str">
             <v>Labor-Handling (30%)</v>
@@ -3193,8 +3193,8 @@
           <cell r="CG7">
             <v>0</v>
           </cell>
-          <cell r="CH7">
-            <v>0</v>
+          <cell r="CH7" t="str">
+            <v>Kurze Hose</v>
           </cell>
         </row>
         <row r="8">
@@ -10383,7 +10383,7 @@
       </c>
       <c r="CH2" s="1">
         <f ca="1">NOW()</f>
-        <v>45818.465395949075</v>
+        <v>45819.727269097224</v>
       </c>
     </row>
     <row r="3" spans="1:87" x14ac:dyDescent="0.25">
@@ -34488,7 +34488,7 @@
       </c>
       <c r="C94">
         <f>[1]Uebertrag!C7</f>
-        <v>1.1333333333333333</v>
+        <v>1.3338333333333334</v>
       </c>
       <c r="D94">
         <f>[1]Uebertrag!D7</f>
@@ -34496,7 +34496,7 @@
       </c>
       <c r="E94">
         <f>[1]Uebertrag!E7</f>
-        <v>1.1333333333333333</v>
+        <v>1.3338333333333334</v>
       </c>
       <c r="F94" t="str">
         <f>[1]Uebertrag!F7</f>
@@ -34760,7 +34760,7 @@
       </c>
       <c r="BS94">
         <f>[1]Uebertrag!BS7</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BT94" t="str">
         <f>[1]Uebertrag!BT7</f>
@@ -34818,9 +34818,9 @@
         <f>[1]Uebertrag!CG7</f>
         <v>0</v>
       </c>
-      <c r="CH94">
+      <c r="CH94" t="str">
         <f>[1]Uebertrag!CH7</f>
-        <v>0</v>
+        <v>Kurze Hose</v>
       </c>
     </row>
     <row r="95" spans="1:86" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Automatisches Update vom 2025-06-16_17-33
</commit_message>
<xml_diff>
--- a/NotenAllSuS.xlsx
+++ b/NotenAllSuS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{379FB828-E368-4B48-8220-804C9F630640}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3210" windowWidth="21600" windowHeight="11385" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
   </bookViews>
   <sheets>
     <sheet name="NotenAllSuS" sheetId="1" r:id="rId1"/>
@@ -4329,7 +4329,7 @@
             <v>0</v>
           </cell>
           <cell r="V3" t="str">
-            <v>W9</v>
+            <v>Fehlerfund</v>
           </cell>
           <cell r="W3">
             <v>0</v>
@@ -4376,8 +4376,8 @@
           <cell r="AK3">
             <v>3</v>
           </cell>
-          <cell r="AL3">
-            <v>7</v>
+          <cell r="AL3" t="str">
+            <v>Elekt. Massenabscheidung</v>
           </cell>
           <cell r="AM3">
             <v>0</v>
@@ -4589,7 +4589,7 @@
             <v>0</v>
           </cell>
           <cell r="V6" t="str">
-            <v>W9</v>
+            <v>Fehlerfund</v>
           </cell>
           <cell r="W6">
             <v>0</v>
@@ -4636,8 +4636,8 @@
           <cell r="AK6">
             <v>5</v>
           </cell>
-          <cell r="AL6">
-            <v>7</v>
+          <cell r="AL6" t="str">
+            <v>Elekt. Massenabscheidung</v>
           </cell>
           <cell r="AM6">
             <v>0</v>
@@ -4792,13 +4792,13 @@
             <v>24_3cCVT AMA N</v>
           </cell>
           <cell r="C8">
-            <v>1.83</v>
+            <v>1.71</v>
           </cell>
           <cell r="D8">
             <v>2.4</v>
           </cell>
           <cell r="E8">
-            <v>2.17</v>
+            <v>2.13</v>
           </cell>
           <cell r="F8" t="str">
             <v>W1</v>
@@ -4849,10 +4849,10 @@
             <v>0</v>
           </cell>
           <cell r="V8" t="str">
-            <v>W9</v>
+            <v>Fehlerfund</v>
           </cell>
           <cell r="W8">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="X8" t="str">
             <v>Mitschrift</v>
@@ -4896,8 +4896,8 @@
           <cell r="AK8">
             <v>5</v>
           </cell>
-          <cell r="AL8">
-            <v>7</v>
+          <cell r="AL8" t="str">
+            <v>Elekt. Massenabscheidung</v>
           </cell>
           <cell r="AM8">
             <v>0</v>
@@ -5109,7 +5109,7 @@
             <v>0</v>
           </cell>
           <cell r="V9" t="str">
-            <v>W9</v>
+            <v>Fehlerfund</v>
           </cell>
           <cell r="W9">
             <v>0</v>
@@ -5156,8 +5156,8 @@
           <cell r="AK9">
             <v>4</v>
           </cell>
-          <cell r="AL9">
-            <v>7</v>
+          <cell r="AL9" t="str">
+            <v>Elekt. Massenabscheidung</v>
           </cell>
           <cell r="AM9">
             <v>0</v>
@@ -5369,7 +5369,7 @@
             <v>0</v>
           </cell>
           <cell r="V11" t="str">
-            <v>W9</v>
+            <v>Fehlerfund</v>
           </cell>
           <cell r="W11">
             <v>0</v>
@@ -5416,8 +5416,8 @@
           <cell r="AK11">
             <v>4</v>
           </cell>
-          <cell r="AL11">
-            <v>7</v>
+          <cell r="AL11" t="str">
+            <v>Elekt. Massenabscheidung</v>
           </cell>
           <cell r="AM11">
             <v>0</v>
@@ -5629,7 +5629,7 @@
             <v>0</v>
           </cell>
           <cell r="V12" t="str">
-            <v>W9</v>
+            <v>Fehlerfund</v>
           </cell>
           <cell r="W12">
             <v>0</v>
@@ -5676,8 +5676,8 @@
           <cell r="AK12">
             <v>5</v>
           </cell>
-          <cell r="AL12">
-            <v>7</v>
+          <cell r="AL12" t="str">
+            <v>Elekt. Massenabscheidung</v>
           </cell>
           <cell r="AM12">
             <v>0</v>
@@ -5889,7 +5889,7 @@
             <v>0</v>
           </cell>
           <cell r="V13" t="str">
-            <v>W9</v>
+            <v>Fehlerfund</v>
           </cell>
           <cell r="W13">
             <v>0</v>
@@ -5936,8 +5936,8 @@
           <cell r="AK13">
             <v>3</v>
           </cell>
-          <cell r="AL13">
-            <v>7</v>
+          <cell r="AL13" t="str">
+            <v>Elekt. Massenabscheidung</v>
           </cell>
           <cell r="AM13">
             <v>0</v>
@@ -6149,7 +6149,7 @@
             <v>0</v>
           </cell>
           <cell r="V15" t="str">
-            <v>W9</v>
+            <v>Fehlerfund</v>
           </cell>
           <cell r="W15">
             <v>0</v>
@@ -6196,8 +6196,8 @@
           <cell r="AK15">
             <v>4</v>
           </cell>
-          <cell r="AL15">
-            <v>7</v>
+          <cell r="AL15" t="str">
+            <v>Elekt. Massenabscheidung</v>
           </cell>
           <cell r="AM15">
             <v>0</v>
@@ -6409,7 +6409,7 @@
             <v>0</v>
           </cell>
           <cell r="V16" t="str">
-            <v>W9</v>
+            <v>Fehlerfund</v>
           </cell>
           <cell r="W16">
             <v>0</v>
@@ -6456,8 +6456,8 @@
           <cell r="AK16">
             <v>5</v>
           </cell>
-          <cell r="AL16">
-            <v>7</v>
+          <cell r="AL16" t="str">
+            <v>Elekt. Massenabscheidung</v>
           </cell>
           <cell r="AM16">
             <v>0</v>
@@ -6669,7 +6669,7 @@
             <v>0</v>
           </cell>
           <cell r="V18" t="str">
-            <v>W9</v>
+            <v>Fehlerfund</v>
           </cell>
           <cell r="W18">
             <v>0</v>
@@ -6716,8 +6716,8 @@
           <cell r="AK18">
             <v>3</v>
           </cell>
-          <cell r="AL18">
-            <v>7</v>
+          <cell r="AL18" t="str">
+            <v>Elekt. Massenabscheidung</v>
           </cell>
           <cell r="AM18">
             <v>0</v>
@@ -6896,13 +6896,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C2">
-            <v>1.75</v>
+            <v>1.67</v>
           </cell>
           <cell r="D2">
-            <v>1.45</v>
+            <v>1.63</v>
           </cell>
           <cell r="E2">
-            <v>1.57</v>
+            <v>1.64</v>
           </cell>
           <cell r="F2" t="str">
             <v>W1</v>
@@ -6935,31 +6935,31 @@
             <v>1</v>
           </cell>
           <cell r="P2" t="str">
-            <v>W6</v>
+            <v>W6+7</v>
           </cell>
           <cell r="Q2">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="R2" t="str">
-            <v>W7</v>
+            <v>W8</v>
           </cell>
           <cell r="S2">
             <v>0</v>
           </cell>
           <cell r="T2" t="str">
-            <v>W8</v>
+            <v>W9</v>
           </cell>
           <cell r="U2">
             <v>0</v>
           </cell>
           <cell r="V2" t="str">
-            <v>W9</v>
+            <v>W10</v>
           </cell>
           <cell r="W2">
             <v>0</v>
           </cell>
           <cell r="X2" t="str">
-            <v>W10</v>
+            <v>Mitschrift</v>
           </cell>
           <cell r="Y2">
             <v>0</v>
@@ -6988,8 +6988,8 @@
           <cell r="AG2">
             <v>3</v>
           </cell>
-          <cell r="AH2">
-            <v>5</v>
+          <cell r="AH2" t="str">
+            <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI2">
             <v>0</v>
@@ -7127,13 +7127,13 @@
             <v>15</v>
           </cell>
           <cell r="CB2">
-            <v>0</v>
+            <v>2</v>
           </cell>
           <cell r="CC2">
-            <v>0</v>
+            <v>13.5</v>
           </cell>
           <cell r="CD2">
-            <v>0</v>
+            <v>16</v>
           </cell>
           <cell r="CE2">
             <v>0</v>
@@ -7153,13 +7153,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C4">
-            <v>1.63</v>
+            <v>1.56</v>
           </cell>
           <cell r="D4">
-            <v>1.1499999999999999</v>
+            <v>1.25</v>
           </cell>
           <cell r="E4">
-            <v>1.34</v>
+            <v>1.37</v>
           </cell>
           <cell r="F4" t="str">
             <v>W1</v>
@@ -7192,31 +7192,31 @@
             <v>1</v>
           </cell>
           <cell r="P4" t="str">
-            <v>W6</v>
+            <v>W6+7</v>
           </cell>
           <cell r="Q4">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="R4" t="str">
-            <v>W7</v>
+            <v>W8</v>
           </cell>
           <cell r="S4">
             <v>0</v>
           </cell>
           <cell r="T4" t="str">
-            <v>W8</v>
+            <v>W9</v>
           </cell>
           <cell r="U4">
             <v>0</v>
           </cell>
           <cell r="V4" t="str">
-            <v>W9</v>
+            <v>W10</v>
           </cell>
           <cell r="W4">
             <v>0</v>
           </cell>
           <cell r="X4" t="str">
-            <v>W10</v>
+            <v>Mitschrift</v>
           </cell>
           <cell r="Y4">
             <v>0</v>
@@ -7245,8 +7245,8 @@
           <cell r="AG4" t="str">
             <v>K</v>
           </cell>
-          <cell r="AH4">
-            <v>5</v>
+          <cell r="AH4" t="str">
+            <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI4">
             <v>0</v>
@@ -7384,13 +7384,13 @@
             <v>15</v>
           </cell>
           <cell r="CB4">
-            <v>0</v>
+            <v>1.44</v>
           </cell>
           <cell r="CC4">
-            <v>0</v>
+            <v>14.5</v>
           </cell>
           <cell r="CD4">
-            <v>0</v>
+            <v>16</v>
           </cell>
           <cell r="CE4">
             <v>0</v>
@@ -7410,13 +7410,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C11">
-            <v>2.38</v>
+            <v>2.2200000000000002</v>
           </cell>
           <cell r="D11">
-            <v>2.67</v>
+            <v>2.5499999999999998</v>
           </cell>
           <cell r="E11">
-            <v>2.5499999999999998</v>
+            <v>2.42</v>
           </cell>
           <cell r="F11" t="str">
             <v>W1</v>
@@ -7449,31 +7449,31 @@
             <v>1</v>
           </cell>
           <cell r="P11" t="str">
-            <v>W6</v>
+            <v>W6+7</v>
           </cell>
           <cell r="Q11">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="R11" t="str">
-            <v>W7</v>
+            <v>W8</v>
           </cell>
           <cell r="S11">
             <v>0</v>
           </cell>
           <cell r="T11" t="str">
-            <v>W8</v>
+            <v>W9</v>
           </cell>
           <cell r="U11">
             <v>0</v>
           </cell>
           <cell r="V11" t="str">
-            <v>W9</v>
+            <v>W10</v>
           </cell>
           <cell r="W11">
             <v>0</v>
           </cell>
           <cell r="X11" t="str">
-            <v>W10</v>
+            <v>Mitschrift</v>
           </cell>
           <cell r="Y11">
             <v>0</v>
@@ -7502,8 +7502,8 @@
           <cell r="AG11">
             <v>3</v>
           </cell>
-          <cell r="AH11">
-            <v>5</v>
+          <cell r="AH11" t="str">
+            <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI11">
             <v>0</v>
@@ -7641,13 +7641,13 @@
             <v>15</v>
           </cell>
           <cell r="CB11">
-            <v>0</v>
+            <v>2.2999999999999998</v>
           </cell>
           <cell r="CC11">
-            <v>0</v>
+            <v>13</v>
           </cell>
           <cell r="CD11">
-            <v>0</v>
+            <v>16</v>
           </cell>
           <cell r="CE11">
             <v>0</v>
@@ -7667,13 +7667,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C12">
-            <v>3.75</v>
+            <v>3.78</v>
           </cell>
           <cell r="D12">
-            <v>5</v>
+            <v>4.57</v>
           </cell>
           <cell r="E12">
-            <v>4.5</v>
+            <v>4.51</v>
           </cell>
           <cell r="F12" t="str">
             <v>W1</v>
@@ -7706,31 +7706,31 @@
             <v>4</v>
           </cell>
           <cell r="P12" t="str">
-            <v>W6</v>
+            <v>W6+7</v>
           </cell>
           <cell r="Q12">
-            <v>0</v>
+            <v>4</v>
           </cell>
           <cell r="R12" t="str">
-            <v>W7</v>
+            <v>W8</v>
           </cell>
           <cell r="S12">
             <v>0</v>
           </cell>
           <cell r="T12" t="str">
-            <v>W8</v>
+            <v>W9</v>
           </cell>
           <cell r="U12">
             <v>0</v>
           </cell>
           <cell r="V12" t="str">
-            <v>W9</v>
+            <v>W10</v>
           </cell>
           <cell r="W12">
             <v>0</v>
           </cell>
           <cell r="X12" t="str">
-            <v>W10</v>
+            <v>Mitschrift</v>
           </cell>
           <cell r="Y12">
             <v>0</v>
@@ -7759,8 +7759,8 @@
           <cell r="AG12">
             <v>5</v>
           </cell>
-          <cell r="AH12">
-            <v>5</v>
+          <cell r="AH12" t="str">
+            <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI12">
             <v>0</v>
@@ -7898,13 +7898,13 @@
             <v>15</v>
           </cell>
           <cell r="CB12">
-            <v>0</v>
+            <v>3.7</v>
           </cell>
           <cell r="CC12">
-            <v>0</v>
+            <v>10</v>
           </cell>
           <cell r="CD12">
-            <v>0</v>
+            <v>16</v>
           </cell>
           <cell r="CE12">
             <v>0</v>
@@ -7916,7 +7916,7 @@
             <v>0</v>
           </cell>
           <cell r="CH12" t="str">
-            <v>Beteiligen Sie sich mehr am Unterricht und Lernen Sie mit. Ich werde Sie in diesem Fach mahnen.</v>
+            <v>Beteiligen Sie sich mehr am Unterricht und Lernen Sie mit.</v>
           </cell>
         </row>
         <row r="14">
@@ -7963,31 +7963,31 @@
             <v>0</v>
           </cell>
           <cell r="P14" t="str">
-            <v>W6</v>
+            <v>W6+7</v>
           </cell>
           <cell r="Q14">
             <v>0</v>
           </cell>
           <cell r="R14" t="str">
-            <v>W7</v>
+            <v>W8</v>
           </cell>
           <cell r="S14">
             <v>0</v>
           </cell>
           <cell r="T14" t="str">
-            <v>W8</v>
+            <v>W9</v>
           </cell>
           <cell r="U14">
             <v>0</v>
           </cell>
           <cell r="V14" t="str">
-            <v>W9</v>
+            <v>W10</v>
           </cell>
           <cell r="W14">
             <v>0</v>
           </cell>
           <cell r="X14" t="str">
-            <v>W10</v>
+            <v>Mitschrift</v>
           </cell>
           <cell r="Y14">
             <v>0</v>
@@ -8016,8 +8016,8 @@
           <cell r="AG14">
             <v>0</v>
           </cell>
-          <cell r="AH14">
-            <v>5</v>
+          <cell r="AH14" t="str">
+            <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI14">
             <v>0</v>
@@ -8161,7 +8161,7 @@
             <v>0</v>
           </cell>
           <cell r="CD14">
-            <v>0</v>
+            <v>16</v>
           </cell>
           <cell r="CE14">
             <v>0</v>
@@ -8181,13 +8181,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C15">
-            <v>2.13</v>
+            <v>2</v>
           </cell>
           <cell r="D15">
-            <v>1.7</v>
+            <v>2.4300000000000002</v>
           </cell>
           <cell r="E15">
-            <v>1.87</v>
+            <v>2.2599999999999998</v>
           </cell>
           <cell r="F15" t="str">
             <v>W1</v>
@@ -8220,31 +8220,31 @@
             <v>1</v>
           </cell>
           <cell r="P15" t="str">
-            <v>W6</v>
+            <v>W6+7</v>
           </cell>
           <cell r="Q15">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="R15" t="str">
-            <v>W7</v>
+            <v>W8</v>
           </cell>
           <cell r="S15">
             <v>0</v>
           </cell>
           <cell r="T15" t="str">
-            <v>W8</v>
+            <v>W9</v>
           </cell>
           <cell r="U15">
             <v>0</v>
           </cell>
           <cell r="V15" t="str">
-            <v>W9</v>
+            <v>W10</v>
           </cell>
           <cell r="W15">
             <v>0</v>
           </cell>
           <cell r="X15" t="str">
-            <v>W10</v>
+            <v>Mitschrift</v>
           </cell>
           <cell r="Y15">
             <v>0</v>
@@ -8273,8 +8273,8 @@
           <cell r="AG15">
             <v>2</v>
           </cell>
-          <cell r="AH15">
-            <v>5</v>
+          <cell r="AH15" t="str">
+            <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI15">
             <v>0</v>
@@ -8412,13 +8412,13 @@
             <v>15</v>
           </cell>
           <cell r="CB15">
-            <v>0</v>
+            <v>3.9</v>
           </cell>
           <cell r="CC15">
-            <v>0</v>
+            <v>9.5</v>
           </cell>
           <cell r="CD15">
-            <v>0</v>
+            <v>16</v>
           </cell>
           <cell r="CE15">
             <v>0</v>
@@ -8438,13 +8438,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C16">
-            <v>3.38</v>
+            <v>3.33</v>
           </cell>
           <cell r="D16">
-            <v>3.35</v>
+            <v>3.9</v>
           </cell>
           <cell r="E16">
-            <v>3.36</v>
+            <v>3.67</v>
           </cell>
           <cell r="F16" t="str">
             <v>W1</v>
@@ -8477,31 +8477,31 @@
             <v>4</v>
           </cell>
           <cell r="P16" t="str">
-            <v>W6</v>
+            <v>W6+7</v>
           </cell>
           <cell r="Q16">
-            <v>0</v>
+            <v>3</v>
           </cell>
           <cell r="R16" t="str">
-            <v>W7</v>
+            <v>W8</v>
           </cell>
           <cell r="S16">
             <v>0</v>
           </cell>
           <cell r="T16" t="str">
-            <v>W8</v>
+            <v>W9</v>
           </cell>
           <cell r="U16">
             <v>0</v>
           </cell>
           <cell r="V16" t="str">
-            <v>W9</v>
+            <v>W10</v>
           </cell>
           <cell r="W16">
             <v>0</v>
           </cell>
           <cell r="X16" t="str">
-            <v>W10</v>
+            <v>Mitschrift</v>
           </cell>
           <cell r="Y16">
             <v>0</v>
@@ -8530,8 +8530,8 @@
           <cell r="AG16">
             <v>5</v>
           </cell>
-          <cell r="AH16">
-            <v>5</v>
+          <cell r="AH16" t="str">
+            <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI16">
             <v>0</v>
@@ -8669,13 +8669,13 @@
             <v>15</v>
           </cell>
           <cell r="CB16">
-            <v>0</v>
+            <v>5</v>
           </cell>
           <cell r="CC16">
-            <v>0</v>
+            <v>7</v>
           </cell>
           <cell r="CD16">
-            <v>0</v>
+            <v>16</v>
           </cell>
           <cell r="CE16">
             <v>0</v>
@@ -8695,13 +8695,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C17">
-            <v>2.88</v>
+            <v>2.78</v>
           </cell>
           <cell r="D17">
-            <v>2.15</v>
+            <v>2.2000000000000002</v>
           </cell>
           <cell r="E17">
-            <v>2.44</v>
+            <v>2.4300000000000002</v>
           </cell>
           <cell r="F17" t="str">
             <v>W1</v>
@@ -8734,31 +8734,31 @@
             <v>3</v>
           </cell>
           <cell r="P17" t="str">
-            <v>W6</v>
+            <v>W6+7</v>
           </cell>
           <cell r="Q17">
-            <v>0</v>
+            <v>2</v>
           </cell>
           <cell r="R17" t="str">
-            <v>W7</v>
+            <v>W8</v>
           </cell>
           <cell r="S17">
             <v>0</v>
           </cell>
           <cell r="T17" t="str">
-            <v>W8</v>
+            <v>W9</v>
           </cell>
           <cell r="U17">
             <v>0</v>
           </cell>
           <cell r="V17" t="str">
-            <v>W9</v>
+            <v>W10</v>
           </cell>
           <cell r="W17">
             <v>0</v>
           </cell>
           <cell r="X17" t="str">
-            <v>W10</v>
+            <v>Mitschrift</v>
           </cell>
           <cell r="Y17">
             <v>0</v>
@@ -8787,8 +8787,8 @@
           <cell r="AG17">
             <v>4</v>
           </cell>
-          <cell r="AH17">
-            <v>5</v>
+          <cell r="AH17" t="str">
+            <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI17">
             <v>0</v>
@@ -8926,13 +8926,13 @@
             <v>15</v>
           </cell>
           <cell r="CB17">
-            <v>0</v>
+            <v>2.2999999999999998</v>
           </cell>
           <cell r="CC17">
-            <v>0</v>
+            <v>13</v>
           </cell>
           <cell r="CD17">
-            <v>0</v>
+            <v>16</v>
           </cell>
           <cell r="CE17">
             <v>0</v>
@@ -8952,13 +8952,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C18">
-            <v>1.78</v>
+            <v>1.8</v>
           </cell>
           <cell r="D18">
-            <v>3</v>
+            <v>2.87</v>
           </cell>
           <cell r="E18">
-            <v>2.5099999999999998</v>
+            <v>2.44</v>
           </cell>
           <cell r="F18" t="str">
             <v>W1</v>
@@ -8991,31 +8991,31 @@
             <v>2</v>
           </cell>
           <cell r="P18" t="str">
-            <v>W6</v>
+            <v>W6+7</v>
           </cell>
           <cell r="Q18">
-            <v>0</v>
+            <v>2</v>
           </cell>
           <cell r="R18" t="str">
-            <v>W7</v>
+            <v>W8</v>
           </cell>
           <cell r="S18">
             <v>0</v>
           </cell>
           <cell r="T18" t="str">
-            <v>W8</v>
+            <v>W9</v>
           </cell>
           <cell r="U18">
             <v>0</v>
           </cell>
           <cell r="V18" t="str">
-            <v>W9</v>
+            <v>W10</v>
           </cell>
           <cell r="W18">
             <v>0</v>
           </cell>
           <cell r="X18" t="str">
-            <v>W10</v>
+            <v>Mitschrift</v>
           </cell>
           <cell r="Y18">
             <v>0</v>
@@ -9044,8 +9044,8 @@
           <cell r="AG18">
             <v>2</v>
           </cell>
-          <cell r="AH18">
-            <v>5</v>
+          <cell r="AH18" t="str">
+            <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI18">
             <v>0</v>
@@ -9183,13 +9183,13 @@
             <v>15</v>
           </cell>
           <cell r="CB18">
-            <v>0</v>
+            <v>2.6</v>
           </cell>
           <cell r="CC18">
-            <v>0</v>
+            <v>12.5</v>
           </cell>
           <cell r="CD18">
-            <v>0</v>
+            <v>16</v>
           </cell>
           <cell r="CE18">
             <v>0</v>
@@ -9209,13 +9209,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C19">
-            <v>2</v>
+            <v>1.88</v>
           </cell>
           <cell r="D19">
-            <v>3.15</v>
+            <v>3.1</v>
           </cell>
           <cell r="E19">
-            <v>2.69</v>
+            <v>2.61</v>
           </cell>
           <cell r="F19" t="str">
             <v>W1</v>
@@ -9248,31 +9248,31 @@
             <v>3</v>
           </cell>
           <cell r="P19" t="str">
-            <v>W6</v>
+            <v>W6+7</v>
           </cell>
           <cell r="Q19">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="R19" t="str">
-            <v>W7</v>
+            <v>W8</v>
           </cell>
           <cell r="S19">
             <v>0</v>
           </cell>
           <cell r="T19" t="str">
-            <v>W8</v>
+            <v>W9</v>
           </cell>
           <cell r="U19">
             <v>0</v>
           </cell>
           <cell r="V19" t="str">
-            <v>W9</v>
+            <v>W10</v>
           </cell>
           <cell r="W19">
             <v>0</v>
           </cell>
           <cell r="X19" t="str">
-            <v>W10</v>
+            <v>Mitschrift</v>
           </cell>
           <cell r="Y19">
             <v>0</v>
@@ -9301,8 +9301,8 @@
           <cell r="AG19">
             <v>3</v>
           </cell>
-          <cell r="AH19">
-            <v>5</v>
+          <cell r="AH19" t="str">
+            <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI19">
             <v>0</v>
@@ -9440,13 +9440,13 @@
             <v>15</v>
           </cell>
           <cell r="CB19">
-            <v>0</v>
+            <v>3</v>
           </cell>
           <cell r="CC19">
-            <v>0</v>
+            <v>11.5</v>
           </cell>
           <cell r="CD19">
-            <v>0</v>
+            <v>16</v>
           </cell>
           <cell r="CE19">
             <v>0</v>
@@ -10383,7 +10383,7 @@
       </c>
       <c r="CH2" s="1">
         <f ca="1">NOW()</f>
-        <v>45819.727269097224</v>
+        <v>45824.727272337965</v>
       </c>
     </row>
     <row r="3" spans="1:87" x14ac:dyDescent="0.25">
@@ -36294,7 +36294,7 @@
       </c>
       <c r="V99" t="str">
         <f>[2]HTMLÜbertrag!V3</f>
-        <v>W9</v>
+        <v>Fehlerfund</v>
       </c>
       <c r="W99">
         <f>[2]HTMLÜbertrag!W3</f>
@@ -36356,9 +36356,9 @@
         <f>[2]HTMLÜbertrag!AK3</f>
         <v>3</v>
       </c>
-      <c r="AL99">
+      <c r="AL99" t="str">
         <f>[2]HTMLÜbertrag!AL3</f>
-        <v>7</v>
+        <v>Elekt. Massenabscheidung</v>
       </c>
       <c r="AM99">
         <f>[2]HTMLÜbertrag!AM3</f>
@@ -36640,7 +36640,7 @@
       </c>
       <c r="V100" t="str">
         <f>[2]HTMLÜbertrag!V6</f>
-        <v>W9</v>
+        <v>Fehlerfund</v>
       </c>
       <c r="W100">
         <f>[2]HTMLÜbertrag!W6</f>
@@ -36702,9 +36702,9 @@
         <f>[2]HTMLÜbertrag!AK6</f>
         <v>5</v>
       </c>
-      <c r="AL100">
+      <c r="AL100" t="str">
         <f>[2]HTMLÜbertrag!AL6</f>
-        <v>7</v>
+        <v>Elekt. Massenabscheidung</v>
       </c>
       <c r="AM100">
         <f>[2]HTMLÜbertrag!AM6</f>
@@ -36910,7 +36910,7 @@
       </c>
       <c r="C101">
         <f>[2]HTMLÜbertrag!C8</f>
-        <v>1.83</v>
+        <v>1.71</v>
       </c>
       <c r="D101">
         <f>[2]HTMLÜbertrag!D8</f>
@@ -36918,7 +36918,7 @@
       </c>
       <c r="E101">
         <f>[2]HTMLÜbertrag!E8</f>
-        <v>2.17</v>
+        <v>2.13</v>
       </c>
       <c r="F101" t="str">
         <f>[2]HTMLÜbertrag!F8</f>
@@ -36986,11 +36986,11 @@
       </c>
       <c r="V101" t="str">
         <f>[2]HTMLÜbertrag!V8</f>
-        <v>W9</v>
+        <v>Fehlerfund</v>
       </c>
       <c r="W101">
         <f>[2]HTMLÜbertrag!W8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X101" t="str">
         <f>[2]HTMLÜbertrag!X8</f>
@@ -37048,9 +37048,9 @@
         <f>[2]HTMLÜbertrag!AK8</f>
         <v>5</v>
       </c>
-      <c r="AL101">
+      <c r="AL101" t="str">
         <f>[2]HTMLÜbertrag!AL8</f>
-        <v>7</v>
+        <v>Elekt. Massenabscheidung</v>
       </c>
       <c r="AM101">
         <f>[2]HTMLÜbertrag!AM8</f>
@@ -37332,7 +37332,7 @@
       </c>
       <c r="V102" t="str">
         <f>[2]HTMLÜbertrag!V9</f>
-        <v>W9</v>
+        <v>Fehlerfund</v>
       </c>
       <c r="W102">
         <f>[2]HTMLÜbertrag!W9</f>
@@ -37394,9 +37394,9 @@
         <f>[2]HTMLÜbertrag!AK9</f>
         <v>4</v>
       </c>
-      <c r="AL102">
+      <c r="AL102" t="str">
         <f>[2]HTMLÜbertrag!AL9</f>
-        <v>7</v>
+        <v>Elekt. Massenabscheidung</v>
       </c>
       <c r="AM102">
         <f>[2]HTMLÜbertrag!AM9</f>
@@ -37678,7 +37678,7 @@
       </c>
       <c r="V103" t="str">
         <f>[2]HTMLÜbertrag!V11</f>
-        <v>W9</v>
+        <v>Fehlerfund</v>
       </c>
       <c r="W103">
         <f>[2]HTMLÜbertrag!W11</f>
@@ -37740,9 +37740,9 @@
         <f>[2]HTMLÜbertrag!AK11</f>
         <v>4</v>
       </c>
-      <c r="AL103">
+      <c r="AL103" t="str">
         <f>[2]HTMLÜbertrag!AL11</f>
-        <v>7</v>
+        <v>Elekt. Massenabscheidung</v>
       </c>
       <c r="AM103">
         <f>[2]HTMLÜbertrag!AM11</f>
@@ -38024,7 +38024,7 @@
       </c>
       <c r="V104" t="str">
         <f>[2]HTMLÜbertrag!V12</f>
-        <v>W9</v>
+        <v>Fehlerfund</v>
       </c>
       <c r="W104">
         <f>[2]HTMLÜbertrag!W12</f>
@@ -38086,9 +38086,9 @@
         <f>[2]HTMLÜbertrag!AK12</f>
         <v>5</v>
       </c>
-      <c r="AL104">
+      <c r="AL104" t="str">
         <f>[2]HTMLÜbertrag!AL12</f>
-        <v>7</v>
+        <v>Elekt. Massenabscheidung</v>
       </c>
       <c r="AM104">
         <f>[2]HTMLÜbertrag!AM12</f>
@@ -38370,7 +38370,7 @@
       </c>
       <c r="V105" t="str">
         <f>[2]HTMLÜbertrag!V13</f>
-        <v>W9</v>
+        <v>Fehlerfund</v>
       </c>
       <c r="W105">
         <f>[2]HTMLÜbertrag!W13</f>
@@ -38432,9 +38432,9 @@
         <f>[2]HTMLÜbertrag!AK13</f>
         <v>3</v>
       </c>
-      <c r="AL105">
+      <c r="AL105" t="str">
         <f>[2]HTMLÜbertrag!AL13</f>
-        <v>7</v>
+        <v>Elekt. Massenabscheidung</v>
       </c>
       <c r="AM105">
         <f>[2]HTMLÜbertrag!AM13</f>
@@ -38716,7 +38716,7 @@
       </c>
       <c r="V106" t="str">
         <f>[2]HTMLÜbertrag!V15</f>
-        <v>W9</v>
+        <v>Fehlerfund</v>
       </c>
       <c r="W106">
         <f>[2]HTMLÜbertrag!W15</f>
@@ -38778,9 +38778,9 @@
         <f>[2]HTMLÜbertrag!AK15</f>
         <v>4</v>
       </c>
-      <c r="AL106">
+      <c r="AL106" t="str">
         <f>[2]HTMLÜbertrag!AL15</f>
-        <v>7</v>
+        <v>Elekt. Massenabscheidung</v>
       </c>
       <c r="AM106">
         <f>[2]HTMLÜbertrag!AM15</f>
@@ -39062,7 +39062,7 @@
       </c>
       <c r="V107" t="str">
         <f>[2]HTMLÜbertrag!V16</f>
-        <v>W9</v>
+        <v>Fehlerfund</v>
       </c>
       <c r="W107">
         <f>[2]HTMLÜbertrag!W16</f>
@@ -39124,9 +39124,9 @@
         <f>[2]HTMLÜbertrag!AK16</f>
         <v>5</v>
       </c>
-      <c r="AL107">
+      <c r="AL107" t="str">
         <f>[2]HTMLÜbertrag!AL16</f>
-        <v>7</v>
+        <v>Elekt. Massenabscheidung</v>
       </c>
       <c r="AM107">
         <f>[2]HTMLÜbertrag!AM16</f>
@@ -39408,7 +39408,7 @@
       </c>
       <c r="V108" t="str">
         <f>[2]HTMLÜbertrag!V18</f>
-        <v>W9</v>
+        <v>Fehlerfund</v>
       </c>
       <c r="W108">
         <f>[2]HTMLÜbertrag!W18</f>
@@ -39470,9 +39470,9 @@
         <f>[2]HTMLÜbertrag!AK18</f>
         <v>3</v>
       </c>
-      <c r="AL108">
+      <c r="AL108" t="str">
         <f>[2]HTMLÜbertrag!AL18</f>
-        <v>7</v>
+        <v>Elekt. Massenabscheidung</v>
       </c>
       <c r="AM108">
         <f>[2]HTMLÜbertrag!AM18</f>
@@ -39677,15 +39677,15 @@
       </c>
       <c r="C109">
         <f>[3]HTMLÜbertrag!C2</f>
-        <v>1.75</v>
+        <v>1.67</v>
       </c>
       <c r="D109">
         <f>[3]HTMLÜbertrag!D2</f>
-        <v>1.45</v>
+        <v>1.63</v>
       </c>
       <c r="E109">
         <f>[3]HTMLÜbertrag!E2</f>
-        <v>1.57</v>
+        <v>1.64</v>
       </c>
       <c r="F109" t="str">
         <f>[3]HTMLÜbertrag!F2</f>
@@ -39729,15 +39729,15 @@
       </c>
       <c r="P109" t="str">
         <f>[3]HTMLÜbertrag!P2</f>
-        <v>W6</v>
+        <v>W6+7</v>
       </c>
       <c r="Q109">
         <f>[3]HTMLÜbertrag!Q2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R109" t="str">
         <f>[3]HTMLÜbertrag!R2</f>
-        <v>W7</v>
+        <v>W8</v>
       </c>
       <c r="S109">
         <f>[3]HTMLÜbertrag!S2</f>
@@ -39745,7 +39745,7 @@
       </c>
       <c r="T109" t="str">
         <f>[3]HTMLÜbertrag!T2</f>
-        <v>W8</v>
+        <v>W9</v>
       </c>
       <c r="U109">
         <f>[3]HTMLÜbertrag!U2</f>
@@ -39753,7 +39753,7 @@
       </c>
       <c r="V109" t="str">
         <f>[3]HTMLÜbertrag!V2</f>
-        <v>W9</v>
+        <v>W10</v>
       </c>
       <c r="W109">
         <f>[3]HTMLÜbertrag!W2</f>
@@ -39761,7 +39761,7 @@
       </c>
       <c r="X109" t="str">
         <f>[3]HTMLÜbertrag!X2</f>
-        <v>W10</v>
+        <v>Mitschrift</v>
       </c>
       <c r="Y109">
         <f>[3]HTMLÜbertrag!Y2</f>
@@ -39799,9 +39799,9 @@
         <f>[3]HTMLÜbertrag!AG2</f>
         <v>3</v>
       </c>
-      <c r="AH109">
+      <c r="AH109" t="str">
         <f>[3]HTMLÜbertrag!AH2</f>
-        <v>5</v>
+        <v>Darstellung v. Anlagen</v>
       </c>
       <c r="AI109">
         <f>[3]HTMLÜbertrag!AI2</f>
@@ -39985,15 +39985,15 @@
       </c>
       <c r="CB109">
         <f>[3]HTMLÜbertrag!CB2</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CC109">
         <f>[3]HTMLÜbertrag!CC2</f>
-        <v>0</v>
+        <v>13.5</v>
       </c>
       <c r="CD109">
         <f>[3]HTMLÜbertrag!CD2</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="CE109">
         <f>[3]HTMLÜbertrag!CE2</f>
@@ -40022,15 +40022,15 @@
       </c>
       <c r="C110">
         <f>[3]HTMLÜbertrag!C4</f>
-        <v>1.63</v>
+        <v>1.56</v>
       </c>
       <c r="D110">
         <f>[3]HTMLÜbertrag!D4</f>
-        <v>1.1499999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="E110">
         <f>[3]HTMLÜbertrag!E4</f>
-        <v>1.34</v>
+        <v>1.37</v>
       </c>
       <c r="F110" t="str">
         <f>[3]HTMLÜbertrag!F4</f>
@@ -40074,15 +40074,15 @@
       </c>
       <c r="P110" t="str">
         <f>[3]HTMLÜbertrag!P4</f>
-        <v>W6</v>
+        <v>W6+7</v>
       </c>
       <c r="Q110">
         <f>[3]HTMLÜbertrag!Q4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R110" t="str">
         <f>[3]HTMLÜbertrag!R4</f>
-        <v>W7</v>
+        <v>W8</v>
       </c>
       <c r="S110">
         <f>[3]HTMLÜbertrag!S4</f>
@@ -40090,7 +40090,7 @@
       </c>
       <c r="T110" t="str">
         <f>[3]HTMLÜbertrag!T4</f>
-        <v>W8</v>
+        <v>W9</v>
       </c>
       <c r="U110">
         <f>[3]HTMLÜbertrag!U4</f>
@@ -40098,7 +40098,7 @@
       </c>
       <c r="V110" t="str">
         <f>[3]HTMLÜbertrag!V4</f>
-        <v>W9</v>
+        <v>W10</v>
       </c>
       <c r="W110">
         <f>[3]HTMLÜbertrag!W4</f>
@@ -40106,7 +40106,7 @@
       </c>
       <c r="X110" t="str">
         <f>[3]HTMLÜbertrag!X4</f>
-        <v>W10</v>
+        <v>Mitschrift</v>
       </c>
       <c r="Y110">
         <f>[3]HTMLÜbertrag!Y4</f>
@@ -40144,9 +40144,9 @@
         <f>[3]HTMLÜbertrag!AG4</f>
         <v>K</v>
       </c>
-      <c r="AH110">
+      <c r="AH110" t="str">
         <f>[3]HTMLÜbertrag!AH4</f>
-        <v>5</v>
+        <v>Darstellung v. Anlagen</v>
       </c>
       <c r="AI110">
         <f>[3]HTMLÜbertrag!AI4</f>
@@ -40330,15 +40330,15 @@
       </c>
       <c r="CB110">
         <f>[3]HTMLÜbertrag!CB4</f>
-        <v>0</v>
+        <v>1.44</v>
       </c>
       <c r="CC110">
         <f>[3]HTMLÜbertrag!CC4</f>
-        <v>0</v>
+        <v>14.5</v>
       </c>
       <c r="CD110">
         <f>[3]HTMLÜbertrag!CD4</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="CE110">
         <f>[3]HTMLÜbertrag!CE4</f>
@@ -40367,15 +40367,15 @@
       </c>
       <c r="C111">
         <f>[3]HTMLÜbertrag!C11</f>
-        <v>2.38</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="D111">
         <f>[3]HTMLÜbertrag!D11</f>
-        <v>2.67</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="E111">
         <f>[3]HTMLÜbertrag!E11</f>
-        <v>2.5499999999999998</v>
+        <v>2.42</v>
       </c>
       <c r="F111" t="str">
         <f>[3]HTMLÜbertrag!F11</f>
@@ -40419,15 +40419,15 @@
       </c>
       <c r="P111" t="str">
         <f>[3]HTMLÜbertrag!P11</f>
-        <v>W6</v>
+        <v>W6+7</v>
       </c>
       <c r="Q111">
         <f>[3]HTMLÜbertrag!Q11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R111" t="str">
         <f>[3]HTMLÜbertrag!R11</f>
-        <v>W7</v>
+        <v>W8</v>
       </c>
       <c r="S111">
         <f>[3]HTMLÜbertrag!S11</f>
@@ -40435,7 +40435,7 @@
       </c>
       <c r="T111" t="str">
         <f>[3]HTMLÜbertrag!T11</f>
-        <v>W8</v>
+        <v>W9</v>
       </c>
       <c r="U111">
         <f>[3]HTMLÜbertrag!U11</f>
@@ -40443,7 +40443,7 @@
       </c>
       <c r="V111" t="str">
         <f>[3]HTMLÜbertrag!V11</f>
-        <v>W9</v>
+        <v>W10</v>
       </c>
       <c r="W111">
         <f>[3]HTMLÜbertrag!W11</f>
@@ -40451,7 +40451,7 @@
       </c>
       <c r="X111" t="str">
         <f>[3]HTMLÜbertrag!X11</f>
-        <v>W10</v>
+        <v>Mitschrift</v>
       </c>
       <c r="Y111">
         <f>[3]HTMLÜbertrag!Y11</f>
@@ -40489,9 +40489,9 @@
         <f>[3]HTMLÜbertrag!AG11</f>
         <v>3</v>
       </c>
-      <c r="AH111">
+      <c r="AH111" t="str">
         <f>[3]HTMLÜbertrag!AH11</f>
-        <v>5</v>
+        <v>Darstellung v. Anlagen</v>
       </c>
       <c r="AI111">
         <f>[3]HTMLÜbertrag!AI11</f>
@@ -40675,15 +40675,15 @@
       </c>
       <c r="CB111">
         <f>[3]HTMLÜbertrag!CB11</f>
-        <v>0</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="CC111">
         <f>[3]HTMLÜbertrag!CC11</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="CD111">
         <f>[3]HTMLÜbertrag!CD11</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="CE111">
         <f>[3]HTMLÜbertrag!CE11</f>
@@ -40712,15 +40712,15 @@
       </c>
       <c r="C112">
         <f>[3]HTMLÜbertrag!C12</f>
-        <v>3.75</v>
+        <v>3.78</v>
       </c>
       <c r="D112">
         <f>[3]HTMLÜbertrag!D12</f>
-        <v>5</v>
+        <v>4.57</v>
       </c>
       <c r="E112">
         <f>[3]HTMLÜbertrag!E12</f>
-        <v>4.5</v>
+        <v>4.51</v>
       </c>
       <c r="F112" t="str">
         <f>[3]HTMLÜbertrag!F12</f>
@@ -40764,15 +40764,15 @@
       </c>
       <c r="P112" t="str">
         <f>[3]HTMLÜbertrag!P12</f>
-        <v>W6</v>
+        <v>W6+7</v>
       </c>
       <c r="Q112">
         <f>[3]HTMLÜbertrag!Q12</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R112" t="str">
         <f>[3]HTMLÜbertrag!R12</f>
-        <v>W7</v>
+        <v>W8</v>
       </c>
       <c r="S112">
         <f>[3]HTMLÜbertrag!S12</f>
@@ -40780,7 +40780,7 @@
       </c>
       <c r="T112" t="str">
         <f>[3]HTMLÜbertrag!T12</f>
-        <v>W8</v>
+        <v>W9</v>
       </c>
       <c r="U112">
         <f>[3]HTMLÜbertrag!U12</f>
@@ -40788,7 +40788,7 @@
       </c>
       <c r="V112" t="str">
         <f>[3]HTMLÜbertrag!V12</f>
-        <v>W9</v>
+        <v>W10</v>
       </c>
       <c r="W112">
         <f>[3]HTMLÜbertrag!W12</f>
@@ -40796,7 +40796,7 @@
       </c>
       <c r="X112" t="str">
         <f>[3]HTMLÜbertrag!X12</f>
-        <v>W10</v>
+        <v>Mitschrift</v>
       </c>
       <c r="Y112">
         <f>[3]HTMLÜbertrag!Y12</f>
@@ -40834,9 +40834,9 @@
         <f>[3]HTMLÜbertrag!AG12</f>
         <v>5</v>
       </c>
-      <c r="AH112">
+      <c r="AH112" t="str">
         <f>[3]HTMLÜbertrag!AH12</f>
-        <v>5</v>
+        <v>Darstellung v. Anlagen</v>
       </c>
       <c r="AI112">
         <f>[3]HTMLÜbertrag!AI12</f>
@@ -41020,15 +41020,15 @@
       </c>
       <c r="CB112">
         <f>[3]HTMLÜbertrag!CB12</f>
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="CC112">
         <f>[3]HTMLÜbertrag!CC12</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="CD112">
         <f>[3]HTMLÜbertrag!CD12</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="CE112">
         <f>[3]HTMLÜbertrag!CE12</f>
@@ -41044,7 +41044,7 @@
       </c>
       <c r="CH112" t="str">
         <f>[3]HTMLÜbertrag!CH12</f>
-        <v>Beteiligen Sie sich mehr am Unterricht und Lernen Sie mit. Ich werde Sie in diesem Fach mahnen.</v>
+        <v>Beteiligen Sie sich mehr am Unterricht und Lernen Sie mit.</v>
       </c>
     </row>
     <row r="113" spans="1:86" x14ac:dyDescent="0.25">
@@ -41109,7 +41109,7 @@
       </c>
       <c r="P113" t="str">
         <f>[3]HTMLÜbertrag!P14</f>
-        <v>W6</v>
+        <v>W6+7</v>
       </c>
       <c r="Q113">
         <f>[3]HTMLÜbertrag!Q14</f>
@@ -41117,7 +41117,7 @@
       </c>
       <c r="R113" t="str">
         <f>[3]HTMLÜbertrag!R14</f>
-        <v>W7</v>
+        <v>W8</v>
       </c>
       <c r="S113">
         <f>[3]HTMLÜbertrag!S14</f>
@@ -41125,7 +41125,7 @@
       </c>
       <c r="T113" t="str">
         <f>[3]HTMLÜbertrag!T14</f>
-        <v>W8</v>
+        <v>W9</v>
       </c>
       <c r="U113">
         <f>[3]HTMLÜbertrag!U14</f>
@@ -41133,7 +41133,7 @@
       </c>
       <c r="V113" t="str">
         <f>[3]HTMLÜbertrag!V14</f>
-        <v>W9</v>
+        <v>W10</v>
       </c>
       <c r="W113">
         <f>[3]HTMLÜbertrag!W14</f>
@@ -41141,7 +41141,7 @@
       </c>
       <c r="X113" t="str">
         <f>[3]HTMLÜbertrag!X14</f>
-        <v>W10</v>
+        <v>Mitschrift</v>
       </c>
       <c r="Y113">
         <f>[3]HTMLÜbertrag!Y14</f>
@@ -41179,9 +41179,9 @@
         <f>[3]HTMLÜbertrag!AG14</f>
         <v>0</v>
       </c>
-      <c r="AH113">
+      <c r="AH113" t="str">
         <f>[3]HTMLÜbertrag!AH14</f>
-        <v>5</v>
+        <v>Darstellung v. Anlagen</v>
       </c>
       <c r="AI113">
         <f>[3]HTMLÜbertrag!AI14</f>
@@ -41373,7 +41373,7 @@
       </c>
       <c r="CD113">
         <f>[3]HTMLÜbertrag!CD14</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="CE113">
         <f>[3]HTMLÜbertrag!CE14</f>
@@ -41402,15 +41402,15 @@
       </c>
       <c r="C114">
         <f>[3]HTMLÜbertrag!C15</f>
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="D114">
         <f>[3]HTMLÜbertrag!D15</f>
-        <v>1.7</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="E114">
         <f>[3]HTMLÜbertrag!E15</f>
-        <v>1.87</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="F114" t="str">
         <f>[3]HTMLÜbertrag!F15</f>
@@ -41454,15 +41454,15 @@
       </c>
       <c r="P114" t="str">
         <f>[3]HTMLÜbertrag!P15</f>
-        <v>W6</v>
+        <v>W6+7</v>
       </c>
       <c r="Q114">
         <f>[3]HTMLÜbertrag!Q15</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R114" t="str">
         <f>[3]HTMLÜbertrag!R15</f>
-        <v>W7</v>
+        <v>W8</v>
       </c>
       <c r="S114">
         <f>[3]HTMLÜbertrag!S15</f>
@@ -41470,7 +41470,7 @@
       </c>
       <c r="T114" t="str">
         <f>[3]HTMLÜbertrag!T15</f>
-        <v>W8</v>
+        <v>W9</v>
       </c>
       <c r="U114">
         <f>[3]HTMLÜbertrag!U15</f>
@@ -41478,7 +41478,7 @@
       </c>
       <c r="V114" t="str">
         <f>[3]HTMLÜbertrag!V15</f>
-        <v>W9</v>
+        <v>W10</v>
       </c>
       <c r="W114">
         <f>[3]HTMLÜbertrag!W15</f>
@@ -41486,7 +41486,7 @@
       </c>
       <c r="X114" t="str">
         <f>[3]HTMLÜbertrag!X15</f>
-        <v>W10</v>
+        <v>Mitschrift</v>
       </c>
       <c r="Y114">
         <f>[3]HTMLÜbertrag!Y15</f>
@@ -41524,9 +41524,9 @@
         <f>[3]HTMLÜbertrag!AG15</f>
         <v>2</v>
       </c>
-      <c r="AH114">
+      <c r="AH114" t="str">
         <f>[3]HTMLÜbertrag!AH15</f>
-        <v>5</v>
+        <v>Darstellung v. Anlagen</v>
       </c>
       <c r="AI114">
         <f>[3]HTMLÜbertrag!AI15</f>
@@ -41710,15 +41710,15 @@
       </c>
       <c r="CB114">
         <f>[3]HTMLÜbertrag!CB15</f>
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="CC114">
         <f>[3]HTMLÜbertrag!CC15</f>
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="CD114">
         <f>[3]HTMLÜbertrag!CD15</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="CE114">
         <f>[3]HTMLÜbertrag!CE15</f>
@@ -41747,15 +41747,15 @@
       </c>
       <c r="C115">
         <f>[3]HTMLÜbertrag!C16</f>
-        <v>3.38</v>
+        <v>3.33</v>
       </c>
       <c r="D115">
         <f>[3]HTMLÜbertrag!D16</f>
-        <v>3.35</v>
+        <v>3.9</v>
       </c>
       <c r="E115">
         <f>[3]HTMLÜbertrag!E16</f>
-        <v>3.36</v>
+        <v>3.67</v>
       </c>
       <c r="F115" t="str">
         <f>[3]HTMLÜbertrag!F16</f>
@@ -41799,15 +41799,15 @@
       </c>
       <c r="P115" t="str">
         <f>[3]HTMLÜbertrag!P16</f>
-        <v>W6</v>
+        <v>W6+7</v>
       </c>
       <c r="Q115">
         <f>[3]HTMLÜbertrag!Q16</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R115" t="str">
         <f>[3]HTMLÜbertrag!R16</f>
-        <v>W7</v>
+        <v>W8</v>
       </c>
       <c r="S115">
         <f>[3]HTMLÜbertrag!S16</f>
@@ -41815,7 +41815,7 @@
       </c>
       <c r="T115" t="str">
         <f>[3]HTMLÜbertrag!T16</f>
-        <v>W8</v>
+        <v>W9</v>
       </c>
       <c r="U115">
         <f>[3]HTMLÜbertrag!U16</f>
@@ -41823,7 +41823,7 @@
       </c>
       <c r="V115" t="str">
         <f>[3]HTMLÜbertrag!V16</f>
-        <v>W9</v>
+        <v>W10</v>
       </c>
       <c r="W115">
         <f>[3]HTMLÜbertrag!W16</f>
@@ -41831,7 +41831,7 @@
       </c>
       <c r="X115" t="str">
         <f>[3]HTMLÜbertrag!X16</f>
-        <v>W10</v>
+        <v>Mitschrift</v>
       </c>
       <c r="Y115">
         <f>[3]HTMLÜbertrag!Y16</f>
@@ -41869,9 +41869,9 @@
         <f>[3]HTMLÜbertrag!AG16</f>
         <v>5</v>
       </c>
-      <c r="AH115">
+      <c r="AH115" t="str">
         <f>[3]HTMLÜbertrag!AH16</f>
-        <v>5</v>
+        <v>Darstellung v. Anlagen</v>
       </c>
       <c r="AI115">
         <f>[3]HTMLÜbertrag!AI16</f>
@@ -42055,15 +42055,15 @@
       </c>
       <c r="CB115">
         <f>[3]HTMLÜbertrag!CB16</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="CC115">
         <f>[3]HTMLÜbertrag!CC16</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="CD115">
         <f>[3]HTMLÜbertrag!CD16</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="CE115">
         <f>[3]HTMLÜbertrag!CE16</f>
@@ -42092,15 +42092,15 @@
       </c>
       <c r="C116">
         <f>[3]HTMLÜbertrag!C17</f>
-        <v>2.88</v>
+        <v>2.78</v>
       </c>
       <c r="D116">
         <f>[3]HTMLÜbertrag!D17</f>
-        <v>2.15</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E116">
         <f>[3]HTMLÜbertrag!E17</f>
-        <v>2.44</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="F116" t="str">
         <f>[3]HTMLÜbertrag!F17</f>
@@ -42144,15 +42144,15 @@
       </c>
       <c r="P116" t="str">
         <f>[3]HTMLÜbertrag!P17</f>
-        <v>W6</v>
+        <v>W6+7</v>
       </c>
       <c r="Q116">
         <f>[3]HTMLÜbertrag!Q17</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R116" t="str">
         <f>[3]HTMLÜbertrag!R17</f>
-        <v>W7</v>
+        <v>W8</v>
       </c>
       <c r="S116">
         <f>[3]HTMLÜbertrag!S17</f>
@@ -42160,7 +42160,7 @@
       </c>
       <c r="T116" t="str">
         <f>[3]HTMLÜbertrag!T17</f>
-        <v>W8</v>
+        <v>W9</v>
       </c>
       <c r="U116">
         <f>[3]HTMLÜbertrag!U17</f>
@@ -42168,7 +42168,7 @@
       </c>
       <c r="V116" t="str">
         <f>[3]HTMLÜbertrag!V17</f>
-        <v>W9</v>
+        <v>W10</v>
       </c>
       <c r="W116">
         <f>[3]HTMLÜbertrag!W17</f>
@@ -42176,7 +42176,7 @@
       </c>
       <c r="X116" t="str">
         <f>[3]HTMLÜbertrag!X17</f>
-        <v>W10</v>
+        <v>Mitschrift</v>
       </c>
       <c r="Y116">
         <f>[3]HTMLÜbertrag!Y17</f>
@@ -42214,9 +42214,9 @@
         <f>[3]HTMLÜbertrag!AG17</f>
         <v>4</v>
       </c>
-      <c r="AH116">
+      <c r="AH116" t="str">
         <f>[3]HTMLÜbertrag!AH17</f>
-        <v>5</v>
+        <v>Darstellung v. Anlagen</v>
       </c>
       <c r="AI116">
         <f>[3]HTMLÜbertrag!AI17</f>
@@ -42400,15 +42400,15 @@
       </c>
       <c r="CB116">
         <f>[3]HTMLÜbertrag!CB17</f>
-        <v>0</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="CC116">
         <f>[3]HTMLÜbertrag!CC17</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="CD116">
         <f>[3]HTMLÜbertrag!CD17</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="CE116">
         <f>[3]HTMLÜbertrag!CE17</f>
@@ -42437,15 +42437,15 @@
       </c>
       <c r="C117">
         <f>[3]HTMLÜbertrag!C18</f>
-        <v>1.78</v>
+        <v>1.8</v>
       </c>
       <c r="D117">
         <f>[3]HTMLÜbertrag!D18</f>
-        <v>3</v>
+        <v>2.87</v>
       </c>
       <c r="E117">
         <f>[3]HTMLÜbertrag!E18</f>
-        <v>2.5099999999999998</v>
+        <v>2.44</v>
       </c>
       <c r="F117" t="str">
         <f>[3]HTMLÜbertrag!F18</f>
@@ -42489,15 +42489,15 @@
       </c>
       <c r="P117" t="str">
         <f>[3]HTMLÜbertrag!P18</f>
-        <v>W6</v>
+        <v>W6+7</v>
       </c>
       <c r="Q117">
         <f>[3]HTMLÜbertrag!Q18</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R117" t="str">
         <f>[3]HTMLÜbertrag!R18</f>
-        <v>W7</v>
+        <v>W8</v>
       </c>
       <c r="S117">
         <f>[3]HTMLÜbertrag!S18</f>
@@ -42505,7 +42505,7 @@
       </c>
       <c r="T117" t="str">
         <f>[3]HTMLÜbertrag!T18</f>
-        <v>W8</v>
+        <v>W9</v>
       </c>
       <c r="U117">
         <f>[3]HTMLÜbertrag!U18</f>
@@ -42513,7 +42513,7 @@
       </c>
       <c r="V117" t="str">
         <f>[3]HTMLÜbertrag!V18</f>
-        <v>W9</v>
+        <v>W10</v>
       </c>
       <c r="W117">
         <f>[3]HTMLÜbertrag!W18</f>
@@ -42521,7 +42521,7 @@
       </c>
       <c r="X117" t="str">
         <f>[3]HTMLÜbertrag!X18</f>
-        <v>W10</v>
+        <v>Mitschrift</v>
       </c>
       <c r="Y117">
         <f>[3]HTMLÜbertrag!Y18</f>
@@ -42559,9 +42559,9 @@
         <f>[3]HTMLÜbertrag!AG18</f>
         <v>2</v>
       </c>
-      <c r="AH117">
+      <c r="AH117" t="str">
         <f>[3]HTMLÜbertrag!AH18</f>
-        <v>5</v>
+        <v>Darstellung v. Anlagen</v>
       </c>
       <c r="AI117">
         <f>[3]HTMLÜbertrag!AI18</f>
@@ -42745,15 +42745,15 @@
       </c>
       <c r="CB117">
         <f>[3]HTMLÜbertrag!CB18</f>
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="CC117">
         <f>[3]HTMLÜbertrag!CC18</f>
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="CD117">
         <f>[3]HTMLÜbertrag!CD18</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="CE117">
         <f>[3]HTMLÜbertrag!CE18</f>
@@ -42782,15 +42782,15 @@
       </c>
       <c r="C118">
         <f>[3]HTMLÜbertrag!C19</f>
-        <v>2</v>
+        <v>1.88</v>
       </c>
       <c r="D118">
         <f>[3]HTMLÜbertrag!D19</f>
-        <v>3.15</v>
+        <v>3.1</v>
       </c>
       <c r="E118">
         <f>[3]HTMLÜbertrag!E19</f>
-        <v>2.69</v>
+        <v>2.61</v>
       </c>
       <c r="F118" t="str">
         <f>[3]HTMLÜbertrag!F19</f>
@@ -42834,15 +42834,15 @@
       </c>
       <c r="P118" t="str">
         <f>[3]HTMLÜbertrag!P19</f>
-        <v>W6</v>
+        <v>W6+7</v>
       </c>
       <c r="Q118">
         <f>[3]HTMLÜbertrag!Q19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R118" t="str">
         <f>[3]HTMLÜbertrag!R19</f>
-        <v>W7</v>
+        <v>W8</v>
       </c>
       <c r="S118">
         <f>[3]HTMLÜbertrag!S19</f>
@@ -42850,7 +42850,7 @@
       </c>
       <c r="T118" t="str">
         <f>[3]HTMLÜbertrag!T19</f>
-        <v>W8</v>
+        <v>W9</v>
       </c>
       <c r="U118">
         <f>[3]HTMLÜbertrag!U19</f>
@@ -42858,7 +42858,7 @@
       </c>
       <c r="V118" t="str">
         <f>[3]HTMLÜbertrag!V19</f>
-        <v>W9</v>
+        <v>W10</v>
       </c>
       <c r="W118">
         <f>[3]HTMLÜbertrag!W19</f>
@@ -42866,7 +42866,7 @@
       </c>
       <c r="X118" t="str">
         <f>[3]HTMLÜbertrag!X19</f>
-        <v>W10</v>
+        <v>Mitschrift</v>
       </c>
       <c r="Y118">
         <f>[3]HTMLÜbertrag!Y19</f>
@@ -42904,9 +42904,9 @@
         <f>[3]HTMLÜbertrag!AG19</f>
         <v>3</v>
       </c>
-      <c r="AH118">
+      <c r="AH118" t="str">
         <f>[3]HTMLÜbertrag!AH19</f>
-        <v>5</v>
+        <v>Darstellung v. Anlagen</v>
       </c>
       <c r="AI118">
         <f>[3]HTMLÜbertrag!AI19</f>
@@ -43090,15 +43090,15 @@
       </c>
       <c r="CB118">
         <f>[3]HTMLÜbertrag!CB19</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="CC118">
         <f>[3]HTMLÜbertrag!CC19</f>
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="CD118">
         <f>[3]HTMLÜbertrag!CD19</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="CE118">
         <f>[3]HTMLÜbertrag!CE19</f>

</xml_diff>

<commit_message>
Automatisches Update vom 2025-06-16_17-53
</commit_message>
<xml_diff>
--- a/NotenAllSuS.xlsx
+++ b/NotenAllSuS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{379FB828-E368-4B48-8220-804C9F630640}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
   </bookViews>
   <sheets>
     <sheet name="NotenAllSuS" sheetId="1" r:id="rId1"/>
@@ -10383,7 +10383,7 @@
       </c>
       <c r="CH2" s="1">
         <f ca="1">NOW()</f>
-        <v>45824.727272337965</v>
+        <v>45824.740749537035</v>
       </c>
     </row>
     <row r="3" spans="1:87" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Automatisches Update vom 2025-06-16_18-13
</commit_message>
<xml_diff>
--- a/NotenAllSuS.xlsx
+++ b/NotenAllSuS.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{B0F7E4B7-2668-4DC5-9A78-CA91221137A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{379FB828-E368-4B48-8220-804C9F630640}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{E9327768-C018-4B40-9D98-76A993AB0B58}"/>
   </bookViews>
   <sheets>
     <sheet name="NotenAllSuS" sheetId="1" r:id="rId1"/>
@@ -6896,13 +6896,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C2">
-            <v>1.67</v>
+            <v>1.6</v>
           </cell>
           <cell r="D2">
             <v>1.63</v>
           </cell>
           <cell r="E2">
-            <v>1.64</v>
+            <v>1.62</v>
           </cell>
           <cell r="F2" t="str">
             <v>W1</v>
@@ -6992,7 +6992,7 @@
             <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI2">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AJ2">
             <v>6</v>
@@ -7153,13 +7153,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C4">
-            <v>1.56</v>
+            <v>1.5</v>
           </cell>
           <cell r="D4">
             <v>1.25</v>
           </cell>
           <cell r="E4">
-            <v>1.37</v>
+            <v>1.35</v>
           </cell>
           <cell r="F4" t="str">
             <v>W1</v>
@@ -7249,7 +7249,7 @@
             <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI4">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AJ4">
             <v>6</v>
@@ -7410,13 +7410,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C11">
-            <v>2.2200000000000002</v>
+            <v>2.2000000000000002</v>
           </cell>
           <cell r="D11">
             <v>2.5499999999999998</v>
           </cell>
           <cell r="E11">
-            <v>2.42</v>
+            <v>2.41</v>
           </cell>
           <cell r="F11" t="str">
             <v>W1</v>
@@ -7452,7 +7452,7 @@
             <v>W6+7</v>
           </cell>
           <cell r="Q11">
-            <v>1</v>
+            <v>2</v>
           </cell>
           <cell r="R11" t="str">
             <v>W8</v>
@@ -7506,7 +7506,7 @@
             <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI11">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AJ11">
             <v>6</v>
@@ -7667,13 +7667,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C12">
-            <v>3.78</v>
+            <v>3.4</v>
           </cell>
           <cell r="D12">
             <v>4.57</v>
           </cell>
           <cell r="E12">
-            <v>4.51</v>
+            <v>4.0999999999999996</v>
           </cell>
           <cell r="F12" t="str">
             <v>W1</v>
@@ -7709,7 +7709,7 @@
             <v>W6+7</v>
           </cell>
           <cell r="Q12">
-            <v>4</v>
+            <v>3</v>
           </cell>
           <cell r="R12" t="str">
             <v>W8</v>
@@ -7763,7 +7763,7 @@
             <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI12">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AJ12">
             <v>6</v>
@@ -8181,13 +8181,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C15">
-            <v>2</v>
+            <v>2.1</v>
           </cell>
           <cell r="D15">
             <v>2.4300000000000002</v>
           </cell>
           <cell r="E15">
-            <v>2.2599999999999998</v>
+            <v>2.2999999999999998</v>
           </cell>
           <cell r="F15" t="str">
             <v>W1</v>
@@ -8277,7 +8277,7 @@
             <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI15">
-            <v>0</v>
+            <v>3</v>
           </cell>
           <cell r="AJ15">
             <v>6</v>
@@ -8438,13 +8438,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C16">
-            <v>3.33</v>
+            <v>3.1</v>
           </cell>
           <cell r="D16">
             <v>3.9</v>
           </cell>
           <cell r="E16">
-            <v>3.67</v>
+            <v>3.58</v>
           </cell>
           <cell r="F16" t="str">
             <v>W1</v>
@@ -8534,7 +8534,7 @@
             <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI16">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AJ16">
             <v>6</v>
@@ -8695,13 +8695,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C17">
-            <v>2.78</v>
+            <v>2.5</v>
           </cell>
           <cell r="D17">
             <v>2.2000000000000002</v>
           </cell>
           <cell r="E17">
-            <v>2.4300000000000002</v>
+            <v>2.3199999999999998</v>
           </cell>
           <cell r="F17" t="str">
             <v>W1</v>
@@ -8737,7 +8737,7 @@
             <v>W6+7</v>
           </cell>
           <cell r="Q17">
-            <v>2</v>
+            <v>1</v>
           </cell>
           <cell r="R17" t="str">
             <v>W8</v>
@@ -8791,7 +8791,7 @@
             <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI17">
-            <v>0</v>
+            <v>1</v>
           </cell>
           <cell r="AJ17">
             <v>6</v>
@@ -8952,13 +8952,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C18">
-            <v>1.8</v>
+            <v>1.82</v>
           </cell>
           <cell r="D18">
             <v>2.87</v>
           </cell>
           <cell r="E18">
-            <v>2.44</v>
+            <v>2.4500000000000002</v>
           </cell>
           <cell r="F18" t="str">
             <v>W1</v>
@@ -9048,7 +9048,7 @@
             <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI18">
-            <v>0</v>
+            <v>2</v>
           </cell>
           <cell r="AJ18">
             <v>6</v>
@@ -9209,13 +9209,13 @@
             <v>VT-N_24 25_3cCVT</v>
           </cell>
           <cell r="C19">
-            <v>1.88</v>
+            <v>2</v>
           </cell>
           <cell r="D19">
             <v>3.1</v>
           </cell>
           <cell r="E19">
-            <v>2.61</v>
+            <v>2.66</v>
           </cell>
           <cell r="F19" t="str">
             <v>W1</v>
@@ -9305,7 +9305,7 @@
             <v>Darstellung v. Anlagen</v>
           </cell>
           <cell r="AI19">
-            <v>0</v>
+            <v>3</v>
           </cell>
           <cell r="AJ19">
             <v>6</v>
@@ -10383,7 +10383,7 @@
       </c>
       <c r="CH2" s="1">
         <f ca="1">NOW()</f>
-        <v>45824.740749537035</v>
+        <v>45824.756728125001</v>
       </c>
     </row>
     <row r="3" spans="1:87" x14ac:dyDescent="0.25">
@@ -39677,7 +39677,7 @@
       </c>
       <c r="C109">
         <f>[3]HTMLÜbertrag!C2</f>
-        <v>1.67</v>
+        <v>1.6</v>
       </c>
       <c r="D109">
         <f>[3]HTMLÜbertrag!D2</f>
@@ -39685,7 +39685,7 @@
       </c>
       <c r="E109">
         <f>[3]HTMLÜbertrag!E2</f>
-        <v>1.64</v>
+        <v>1.62</v>
       </c>
       <c r="F109" t="str">
         <f>[3]HTMLÜbertrag!F2</f>
@@ -39805,7 +39805,7 @@
       </c>
       <c r="AI109">
         <f>[3]HTMLÜbertrag!AI2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ109">
         <f>[3]HTMLÜbertrag!AJ2</f>
@@ -40022,7 +40022,7 @@
       </c>
       <c r="C110">
         <f>[3]HTMLÜbertrag!C4</f>
-        <v>1.56</v>
+        <v>1.5</v>
       </c>
       <c r="D110">
         <f>[3]HTMLÜbertrag!D4</f>
@@ -40030,7 +40030,7 @@
       </c>
       <c r="E110">
         <f>[3]HTMLÜbertrag!E4</f>
-        <v>1.37</v>
+        <v>1.35</v>
       </c>
       <c r="F110" t="str">
         <f>[3]HTMLÜbertrag!F4</f>
@@ -40150,7 +40150,7 @@
       </c>
       <c r="AI110">
         <f>[3]HTMLÜbertrag!AI4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ110">
         <f>[3]HTMLÜbertrag!AJ4</f>
@@ -40367,7 +40367,7 @@
       </c>
       <c r="C111">
         <f>[3]HTMLÜbertrag!C11</f>
-        <v>2.2200000000000002</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D111">
         <f>[3]HTMLÜbertrag!D11</f>
@@ -40375,7 +40375,7 @@
       </c>
       <c r="E111">
         <f>[3]HTMLÜbertrag!E11</f>
-        <v>2.42</v>
+        <v>2.41</v>
       </c>
       <c r="F111" t="str">
         <f>[3]HTMLÜbertrag!F11</f>
@@ -40423,7 +40423,7 @@
       </c>
       <c r="Q111">
         <f>[3]HTMLÜbertrag!Q11</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R111" t="str">
         <f>[3]HTMLÜbertrag!R11</f>
@@ -40495,7 +40495,7 @@
       </c>
       <c r="AI111">
         <f>[3]HTMLÜbertrag!AI11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ111">
         <f>[3]HTMLÜbertrag!AJ11</f>
@@ -40712,7 +40712,7 @@
       </c>
       <c r="C112">
         <f>[3]HTMLÜbertrag!C12</f>
-        <v>3.78</v>
+        <v>3.4</v>
       </c>
       <c r="D112">
         <f>[3]HTMLÜbertrag!D12</f>
@@ -40720,7 +40720,7 @@
       </c>
       <c r="E112">
         <f>[3]HTMLÜbertrag!E12</f>
-        <v>4.51</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F112" t="str">
         <f>[3]HTMLÜbertrag!F12</f>
@@ -40768,7 +40768,7 @@
       </c>
       <c r="Q112">
         <f>[3]HTMLÜbertrag!Q12</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R112" t="str">
         <f>[3]HTMLÜbertrag!R12</f>
@@ -40840,7 +40840,7 @@
       </c>
       <c r="AI112">
         <f>[3]HTMLÜbertrag!AI12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ112">
         <f>[3]HTMLÜbertrag!AJ12</f>
@@ -41402,7 +41402,7 @@
       </c>
       <c r="C114">
         <f>[3]HTMLÜbertrag!C15</f>
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="D114">
         <f>[3]HTMLÜbertrag!D15</f>
@@ -41410,7 +41410,7 @@
       </c>
       <c r="E114">
         <f>[3]HTMLÜbertrag!E15</f>
-        <v>2.2599999999999998</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F114" t="str">
         <f>[3]HTMLÜbertrag!F15</f>
@@ -41530,7 +41530,7 @@
       </c>
       <c r="AI114">
         <f>[3]HTMLÜbertrag!AI15</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ114">
         <f>[3]HTMLÜbertrag!AJ15</f>
@@ -41747,7 +41747,7 @@
       </c>
       <c r="C115">
         <f>[3]HTMLÜbertrag!C16</f>
-        <v>3.33</v>
+        <v>3.1</v>
       </c>
       <c r="D115">
         <f>[3]HTMLÜbertrag!D16</f>
@@ -41755,7 +41755,7 @@
       </c>
       <c r="E115">
         <f>[3]HTMLÜbertrag!E16</f>
-        <v>3.67</v>
+        <v>3.58</v>
       </c>
       <c r="F115" t="str">
         <f>[3]HTMLÜbertrag!F16</f>
@@ -41875,7 +41875,7 @@
       </c>
       <c r="AI115">
         <f>[3]HTMLÜbertrag!AI16</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ115">
         <f>[3]HTMLÜbertrag!AJ16</f>
@@ -42092,7 +42092,7 @@
       </c>
       <c r="C116">
         <f>[3]HTMLÜbertrag!C17</f>
-        <v>2.78</v>
+        <v>2.5</v>
       </c>
       <c r="D116">
         <f>[3]HTMLÜbertrag!D17</f>
@@ -42100,7 +42100,7 @@
       </c>
       <c r="E116">
         <f>[3]HTMLÜbertrag!E17</f>
-        <v>2.4300000000000002</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="F116" t="str">
         <f>[3]HTMLÜbertrag!F17</f>
@@ -42148,7 +42148,7 @@
       </c>
       <c r="Q116">
         <f>[3]HTMLÜbertrag!Q17</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R116" t="str">
         <f>[3]HTMLÜbertrag!R17</f>
@@ -42220,7 +42220,7 @@
       </c>
       <c r="AI116">
         <f>[3]HTMLÜbertrag!AI17</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ116">
         <f>[3]HTMLÜbertrag!AJ17</f>
@@ -42437,7 +42437,7 @@
       </c>
       <c r="C117">
         <f>[3]HTMLÜbertrag!C18</f>
-        <v>1.8</v>
+        <v>1.82</v>
       </c>
       <c r="D117">
         <f>[3]HTMLÜbertrag!D18</f>
@@ -42445,7 +42445,7 @@
       </c>
       <c r="E117">
         <f>[3]HTMLÜbertrag!E18</f>
-        <v>2.44</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="F117" t="str">
         <f>[3]HTMLÜbertrag!F18</f>
@@ -42565,7 +42565,7 @@
       </c>
       <c r="AI117">
         <f>[3]HTMLÜbertrag!AI18</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ117">
         <f>[3]HTMLÜbertrag!AJ18</f>
@@ -42782,7 +42782,7 @@
       </c>
       <c r="C118">
         <f>[3]HTMLÜbertrag!C19</f>
-        <v>1.88</v>
+        <v>2</v>
       </c>
       <c r="D118">
         <f>[3]HTMLÜbertrag!D19</f>
@@ -42790,7 +42790,7 @@
       </c>
       <c r="E118">
         <f>[3]HTMLÜbertrag!E19</f>
-        <v>2.61</v>
+        <v>2.66</v>
       </c>
       <c r="F118" t="str">
         <f>[3]HTMLÜbertrag!F19</f>
@@ -42910,7 +42910,7 @@
       </c>
       <c r="AI118">
         <f>[3]HTMLÜbertrag!AI19</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ118">
         <f>[3]HTMLÜbertrag!AJ19</f>

</xml_diff>

<commit_message>
Automatisches Update vom 2025-06-17_17-03
</commit_message>
<xml_diff>
--- a/NotenAllSuS.xlsx
+++ b/NotenAllSuS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9467,10 +9467,6 @@
 </externalLink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -9790,18 +9786,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9400B600-DABD-46EA-8221-46FAC4AE4807}">
   <dimension ref="A1:CI120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U88" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AH100" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.43359375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="14.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10061,7 +10057,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>101010</v>
       </c>
@@ -10383,10 +10379,10 @@
       </c>
       <c r="CH2" s="1">
         <f ca="1">NOW()</f>
-        <v>45824.756728125001</v>
+        <v>45825.576440856479</v>
       </c>
     </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>101010</v>
       </c>
@@ -10647,7 +10643,7 @@
       </c>
       <c r="CI3" s="1"/>
     </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>101010</v>
       </c>
@@ -10907,7 +10903,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>238868</v>
       </c>
@@ -11167,7 +11163,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>239513</v>
       </c>
@@ -11427,7 +11423,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>238869</v>
       </c>
@@ -11687,7 +11683,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>238938</v>
       </c>
@@ -11947,7 +11943,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>235241</v>
       </c>
@@ -12207,7 +12203,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>234202</v>
       </c>
@@ -12467,7 +12463,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>239517</v>
       </c>
@@ -12727,7 +12723,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>235188</v>
       </c>
@@ -12987,7 +12983,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>238873</v>
       </c>
@@ -13247,7 +13243,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>235970</v>
       </c>
@@ -13507,7 +13503,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>233683</v>
       </c>
@@ -13767,7 +13763,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:87" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>238629</v>
       </c>
@@ -14027,7 +14023,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="17" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>235163</v>
       </c>
@@ -14287,7 +14283,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>236320</v>
       </c>
@@ -14547,7 +14543,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="19" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>235239</v>
       </c>
@@ -14807,7 +14803,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>240757</v>
       </c>
@@ -15067,7 +15063,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="21" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>241467</v>
       </c>
@@ -15327,7 +15323,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="22" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>227176</v>
       </c>
@@ -15587,7 +15583,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>237814</v>
       </c>
@@ -15847,7 +15843,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>234162</v>
       </c>
@@ -16107,7 +16103,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="25" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>234166</v>
       </c>
@@ -16367,7 +16363,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>234165</v>
       </c>
@@ -16627,7 +16623,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>234159</v>
       </c>
@@ -16887,7 +16883,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>234146</v>
       </c>
@@ -17147,7 +17143,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>234156</v>
       </c>
@@ -17407,7 +17403,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="30" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>234303</v>
       </c>
@@ -17667,7 +17663,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="31" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>234160</v>
       </c>
@@ -17927,7 +17923,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>225611</v>
       </c>
@@ -18187,7 +18183,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="33" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>234157</v>
       </c>
@@ -18447,7 +18443,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>234158</v>
       </c>
@@ -18707,7 +18703,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="35" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>234155</v>
       </c>
@@ -18967,7 +18963,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>234147</v>
       </c>
@@ -19227,7 +19223,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>234144</v>
       </c>
@@ -19487,7 +19483,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>242412</v>
       </c>
@@ -19747,7 +19743,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="39" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>241867</v>
       </c>
@@ -20007,7 +20003,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="40" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>242615</v>
       </c>
@@ -20267,7 +20263,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="41" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>236774</v>
       </c>
@@ -20527,7 +20523,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="42" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>242616</v>
       </c>
@@ -20787,7 +20783,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="43" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>242617</v>
       </c>
@@ -21047,7 +21043,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="44" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>727090</v>
       </c>
@@ -21307,7 +21303,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="45" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>235211</v>
       </c>
@@ -21567,7 +21563,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="46" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>241945</v>
       </c>
@@ -21827,7 +21823,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>238493</v>
       </c>
@@ -22087,7 +22083,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="48" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>242050</v>
       </c>
@@ -22347,7 +22343,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="49" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>238954</v>
       </c>
@@ -22607,7 +22603,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="50" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>239023</v>
       </c>
@@ -22867,7 +22863,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="51" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>238267</v>
       </c>
@@ -23127,7 +23123,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>239024</v>
       </c>
@@ -23387,7 +23383,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="53" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>238314</v>
       </c>
@@ -23647,7 +23643,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="54" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>247308</v>
       </c>
@@ -23907,7 +23903,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="55" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>240051</v>
       </c>
@@ -24167,7 +24163,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="56" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>246501</v>
       </c>
@@ -24427,7 +24423,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="57" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>245566</v>
       </c>
@@ -24687,7 +24683,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="58" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>245509</v>
       </c>
@@ -24947,7 +24943,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="59" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>245510</v>
       </c>
@@ -25207,7 +25203,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="60" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>241923</v>
       </c>
@@ -25467,7 +25463,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="61" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>238486</v>
       </c>
@@ -25727,7 +25723,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="62" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>243487</v>
       </c>
@@ -25987,7 +25983,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="63" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>234145</v>
       </c>
@@ -26247,7 +26243,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="64" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>225004</v>
       </c>
@@ -26507,7 +26503,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="65" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>244511</v>
       </c>
@@ -26767,7 +26763,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="66" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>224044</v>
       </c>
@@ -27027,7 +27023,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="67" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>241871</v>
       </c>
@@ -27287,7 +27283,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="68" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>242618</v>
       </c>
@@ -27547,7 +27543,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="69" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>245041</v>
       </c>
@@ -27807,7 +27803,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="70" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>242619</v>
       </c>
@@ -28067,7 +28063,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="71" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>242620</v>
       </c>
@@ -28327,7 +28323,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="72" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>242622</v>
       </c>
@@ -28587,7 +28583,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="73" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>242621</v>
       </c>
@@ -28847,7 +28843,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="74" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>242623</v>
       </c>
@@ -29107,7 +29103,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="75" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>241872</v>
       </c>
@@ -29367,7 +29363,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="76" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>242625</v>
       </c>
@@ -29627,7 +29623,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="77" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>244014</v>
       </c>
@@ -29887,7 +29883,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="78" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>242627</v>
       </c>
@@ -30147,7 +30143,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="79" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>242631</v>
       </c>
@@ -30407,7 +30403,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="80" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>243487</v>
       </c>
@@ -30667,7 +30663,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="81" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>244511</v>
       </c>
@@ -30927,7 +30923,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="82" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>242618</v>
       </c>
@@ -31187,7 +31183,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="83" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>245041</v>
       </c>
@@ -31447,7 +31443,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="84" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>242619</v>
       </c>
@@ -31707,7 +31703,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="85" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>242622</v>
       </c>
@@ -31967,7 +31963,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="86" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>242621</v>
       </c>
@@ -32227,7 +32223,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="87" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>242623</v>
       </c>
@@ -32487,7 +32483,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="88" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>242631</v>
       </c>
@@ -32747,7 +32743,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="89" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A89">
         <f>[1]Uebertrag!A2</f>
         <v>204606</v>
@@ -33093,7 +33089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A90">
         <f>[1]Uebertrag!A3</f>
         <v>225128</v>
@@ -33439,7 +33435,7 @@
         <v>Ol zu spät</v>
       </c>
     </row>
-    <row r="91" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A91">
         <f>[1]Uebertrag!A4</f>
         <v>229524</v>
@@ -33785,7 +33781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A92">
         <f>[1]Uebertrag!A5</f>
         <v>225129</v>
@@ -34131,7 +34127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A93">
         <f>[1]Uebertrag!A6</f>
         <v>228179</v>
@@ -34477,7 +34473,7 @@
         <v>Abgabe Photometer fehlt</v>
       </c>
     </row>
-    <row r="94" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A94">
         <f>[1]Uebertrag!A7</f>
         <v>227298</v>
@@ -34823,7 +34819,7 @@
         <v>Kurze Hose</v>
       </c>
     </row>
-    <row r="95" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A95">
         <f>[1]Uebertrag!A8</f>
         <v>225126</v>
@@ -35169,7 +35165,7 @@
         <v>Kaugummi, PSA!; Öl nicht abgegeben</v>
       </c>
     </row>
-    <row r="96" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A96">
         <f>[1]Uebertrag!A9</f>
         <v>226369</v>
@@ -35515,7 +35511,7 @@
         <v>Abgabe Photometer, Polarimetrie fehlt, Unsachgemäßer Aufbau + Nichtbeachten grundlegender Sicherheitsvorgaben (dichte Schliffverbindungen, sichere Befestigung). Fehlende Eigenkontrolle vor Versuchsbeginn.  Schaffung einer vermeidbaren Gefahrensituation durch Austritt brennbarer Dämpfe und Überhitzung.</v>
       </c>
     </row>
-    <row r="97" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A97">
         <f>[1]Uebertrag!A10</f>
         <v>226368</v>
@@ -35861,7 +35857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A98">
         <f>[1]Uebertrag!A11</f>
         <v>228085</v>
@@ -36207,7 +36203,7 @@
         <v>Acetylsalizylsäure fehlerhafte Abgabe daher noch nicht bewertet</v>
       </c>
     </row>
-    <row r="99" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A99">
         <f>[2]HTMLÜbertrag!A3</f>
         <v>225936</v>
@@ -36553,7 +36549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A100">
         <f>[2]HTMLÜbertrag!A6</f>
         <v>225954</v>
@@ -36899,7 +36895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A101">
         <f>[2]HTMLÜbertrag!A8</f>
         <v>225939</v>
@@ -37245,7 +37241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A102">
         <f>[2]HTMLÜbertrag!A9</f>
         <v>226813</v>
@@ -37591,7 +37587,7 @@
         <v>Mitschrift sehr gut</v>
       </c>
     </row>
-    <row r="103" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A103">
         <f>[2]HTMLÜbertrag!A11</f>
         <v>225129</v>
@@ -37937,7 +37933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A104">
         <f>[2]HTMLÜbertrag!A12</f>
         <v>228179</v>
@@ -38283,7 +38279,7 @@
         <v>BSP v S. 298+299 fehlen,</v>
       </c>
     </row>
-    <row r="105" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A105">
         <f>[2]HTMLÜbertrag!A13</f>
         <v>225935</v>
@@ -38629,7 +38625,7 @@
         <v>Mitschrift sehr gut</v>
       </c>
     </row>
-    <row r="106" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A106">
         <f>[2]HTMLÜbertrag!A15</f>
         <v>225934</v>
@@ -38975,7 +38971,7 @@
         <v>Mitschrift sehr gut</v>
       </c>
     </row>
-    <row r="107" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A107">
         <f>[2]HTMLÜbertrag!A16</f>
         <v>225126</v>
@@ -39321,7 +39317,7 @@
         <v>Mitschrift in Ordnung</v>
       </c>
     </row>
-    <row r="108" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A108">
         <f>[2]HTMLÜbertrag!A18</f>
         <v>225955</v>
@@ -39667,7 +39663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>204606</v>
       </c>
@@ -40012,7 +40008,7 @@
         <v xml:space="preserve">Motivierter Schüler mit guten Fragen. Entspannen Sie sich und bleiben Sie ehrgeizig. </v>
       </c>
     </row>
-    <row r="110" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>225128</v>
       </c>
@@ -40357,7 +40353,7 @@
         <v>Beteiligt sich oft während des Unterrichts, oft fehlt aber der Feinschliff bei den Aussagen zu einer MA Note 1. Lernen Sie mit.</v>
       </c>
     </row>
-    <row r="111" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>225129</v>
       </c>
@@ -40702,7 +40698,7 @@
         <v>Gute leistung beim zweiten Test! Lernen Sie mit.</v>
       </c>
     </row>
-    <row r="112" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>228179</v>
       </c>
@@ -41047,7 +41043,7 @@
         <v>Beteiligen Sie sich mehr am Unterricht und Lernen Sie mit.</v>
       </c>
     </row>
-    <row r="113" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>227298</v>
       </c>
@@ -41392,7 +41388,7 @@
         <v xml:space="preserve">Aufgestufft. Ihre Formulierung und Kombinationen sind gut. Versuchen Sie bei der Sache zu bleiben. </v>
       </c>
     </row>
-    <row r="114" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>225934</v>
       </c>
@@ -41737,7 +41733,7 @@
         <v>Sie sind bemüht. Alernen Sie mit und genauer.</v>
       </c>
     </row>
-    <row r="115" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>225126</v>
       </c>
@@ -42082,7 +42078,7 @@
         <v>Bitte lernen Sie mit +genauer</v>
       </c>
     </row>
-    <row r="116" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>226369</v>
       </c>
@@ -42427,7 +42423,7 @@
         <v>Oft haben Sie wirklich gute Antworten auf meine Fragen. Trauen Sie sich mehr zu! Versuchen Sie täglich VT zu lernen</v>
       </c>
     </row>
-    <row r="117" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>225955</v>
       </c>
@@ -42772,7 +42768,7 @@
         <v>Die Antworten während des Unterrichts sind oft noch zu wenig genau für eine 1 in der MA</v>
       </c>
     </row>
-    <row r="118" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:86" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>226368</v>
       </c>
@@ -43117,7 +43113,7 @@
         <v>Formulierungskönig! Lernen Sie mit und genau.</v>
       </c>
     </row>
-    <row r="120" spans="1:86" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:86" x14ac:dyDescent="0.2">
       <c r="B120" s="1"/>
     </row>
   </sheetData>
@@ -43134,4 +43130,10 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/DataMashup"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{98442417-ad21-457c-b0dc-ef86207ac051}" enabled="0" method="" siteId="{98442417-ad21-457c-b0dc-ef86207ac051}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>